<commit_message>
Kleine Anpassung in Zeile 5 war keine Validation
</commit_message>
<xml_diff>
--- a/Documents/FragenTemplate.xlsx
+++ b/Documents/FragenTemplate.xlsx
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
   <si>
     <t>Unterkategorie</t>
   </si>
@@ -788,7 +788,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -854,6 +854,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
@@ -890,9 +893,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>2969100</xdr:colOff>
+          <xdr:colOff>2971800</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>442500</xdr:rowOff>
+          <xdr:rowOff>438150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -922,7 +925,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -949,9 +952,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>2969100</xdr:colOff>
+          <xdr:colOff>2971800</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>728250</xdr:rowOff>
+          <xdr:rowOff>723900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -981,7 +984,7 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="de-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
@@ -1361,8 +1364,8 @@
   <dimension ref="A1:BF202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="3" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H193" sqref="H193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,12 +1653,22 @@
       <c r="BF4" s="22"/>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="F5" s="5"/>
+      <c r="A5" s="3" t="str">
+        <f>K3</f>
+        <v>Antwortmöglichkeit3 *</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="F5" s="15"/>
+      <c r="G5"/>
+      <c r="I5"/>
+      <c r="K5"/>
+      <c r="M5"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
-        <f t="shared" ref="A6:A68" si="0">K3</f>
-        <v>Antwortmöglichkeit3 *</v>
+        <f>K202</f>
+        <v>Betriebwirtschaftslehre</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -1666,24 +1679,24 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="str">
-        <f>K202</f>
-        <v>Betriebwirtschaftslehre</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="F7" s="15"/>
-      <c r="G7"/>
-      <c r="I7"/>
-      <c r="K7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="e">
+      <c r="A7" s="3" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" ref="A8:A67" si="0">K5</f>
+        <v>0</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="F8" s="15"/>
+      <c r="G8"/>
+      <c r="I8"/>
+      <c r="K8"/>
+      <c r="M8"/>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1692,11 +1705,31 @@
       </c>
       <c r="C9"/>
       <c r="D9"/>
+      <c r="E9" s="2" t="str">
+        <f t="shared" ref="E9:E67" si="1">IF(ISBLANK(F9)=TRUE,"",IF(COUNTIF(H9,"richtig")+COUNTIF(J9,"richtig")+COUNTIF(L9,"richtig")+COUNTIF(N9,"richtig")&gt;1,"ja","nein"))</f>
+        <v/>
+      </c>
       <c r="F9" s="15"/>
       <c r="G9"/>
+      <c r="H9" s="2" t="str">
+        <f>IF(ISBLANK($F9)=TRUE,"",IF(ISNUMBER(FIND(H$2,VLOOKUP($F9,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
+        <v/>
+      </c>
       <c r="I9"/>
+      <c r="J9" s="2" t="str">
+        <f>IF(ISBLANK($F9)=TRUE,"",IF(ISNUMBER(FIND(J$2,VLOOKUP($F9,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
+        <v/>
+      </c>
       <c r="K9"/>
+      <c r="L9" s="2" t="str">
+        <f>IF(ISBLANK($F9)=TRUE,"",IF(ISNUMBER(FIND(L$2,VLOOKUP($F9,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
+        <v/>
+      </c>
       <c r="M9"/>
+      <c r="N9" s="20" t="str">
+        <f>IF(ISBLANK($F9)=TRUE,"",IF(ISNUMBER(FIND(N$2,VLOOKUP($F9,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1706,7 +1739,7 @@
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10" s="2" t="str">
-        <f t="shared" ref="E10:E68" si="1">IF(ISBLANK(F10)=TRUE,"",IF(COUNTIF(H10,"richtig")+COUNTIF(J10,"richtig")+COUNTIF(L10,"richtig")+COUNTIF(N10,"richtig")&gt;1,"ja","nein"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="F10" s="15"/>
@@ -3614,13 +3647,13 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A68:A131" si="2">K65</f>
         <v>0</v>
       </c>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E68:E128" si="3">IF(ISBLANK(F68)=TRUE,"",IF(COUNTIF(H68,"richtig")+COUNTIF(J68,"richtig")+COUNTIF(L68,"richtig")+COUNTIF(N68,"richtig")&gt;1,"ja","nein"))</f>
         <v/>
       </c>
       <c r="F68" s="15"/>
@@ -3647,13 +3680,13 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <f t="shared" ref="A69:A132" si="2">K66</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69" s="2" t="str">
-        <f t="shared" ref="E69:E129" si="3">IF(ISBLANK(F69)=TRUE,"",IF(COUNTIF(H69,"richtig")+COUNTIF(J69,"richtig")+COUNTIF(L69,"richtig")+COUNTIF(N69,"richtig")&gt;1,"ja","nein"))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F69" s="15"/>
@@ -4290,10 +4323,6 @@
         <v/>
       </c>
       <c r="I88"/>
-      <c r="J88" s="2" t="str">
-        <f>IF(ISBLANK($F88)=TRUE,"",IF(ISNUMBER(FIND(J$2,VLOOKUP($F88,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v/>
-      </c>
       <c r="K88"/>
       <c r="L88" s="2" t="str">
         <f>IF(ISBLANK($F88)=TRUE,"",IF(ISNUMBER(FIND(L$2,VLOOKUP($F88,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
@@ -4469,15 +4498,7 @@
       </c>
       <c r="I94"/>
       <c r="K94"/>
-      <c r="L94" s="2" t="str">
-        <f>IF(ISBLANK($F94)=TRUE,"",IF(ISNUMBER(FIND(L$2,VLOOKUP($F94,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v/>
-      </c>
       <c r="M94"/>
-      <c r="N94" s="20" t="str">
-        <f>IF(ISBLANK($F94)=TRUE,"",IF(ISNUMBER(FIND(N$2,VLOOKUP($F94,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v/>
-      </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
@@ -4555,10 +4576,6 @@
       </c>
       <c r="F98" s="15"/>
       <c r="G98"/>
-      <c r="H98" s="2" t="str">
-        <f>IF(ISBLANK($F98)=TRUE,"",IF(ISNUMBER(FIND(H$2,VLOOKUP($F98,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v/>
-      </c>
       <c r="I98"/>
       <c r="K98"/>
       <c r="M98"/>
@@ -4620,7 +4637,6 @@
         <v>0</v>
       </c>
       <c r="C102"/>
-      <c r="D102"/>
       <c r="E102" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5053,10 +5069,6 @@
         <v>0</v>
       </c>
       <c r="C129"/>
-      <c r="E129" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="F129" s="15"/>
       <c r="G129"/>
       <c r="I129"/>
@@ -5089,7 +5101,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A132:A193" si="4">K129</f>
         <v>0</v>
       </c>
       <c r="C132"/>
@@ -5101,7 +5113,7 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
-        <f t="shared" ref="A133:A196" si="4">K130</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C133"/>
@@ -5200,12 +5212,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C141"/>
-      <c r="F141" s="15"/>
-      <c r="G141"/>
-      <c r="I141"/>
-      <c r="K141"/>
-      <c r="M141"/>
+      <c r="F141" s="5"/>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
@@ -5572,36 +5579,36 @@
       <c r="F193" s="5"/>
     </row>
     <row r="194" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A194" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F194" s="5"/>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
+      <c r="I194" s="6"/>
+      <c r="K194" s="6"/>
+      <c r="M194" s="6"/>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
-        <f t="shared" si="4"/>
+        <f>K191</f>
         <v>0</v>
       </c>
       <c r="F195" s="5"/>
     </row>
     <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
-        <f t="shared" si="4"/>
+        <f>K192</f>
         <v>0</v>
       </c>
       <c r="F196" s="5"/>
     </row>
     <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
-        <f t="shared" ref="A197:A200" si="5">K194</f>
+        <f>K193</f>
         <v>0</v>
       </c>
       <c r="F197" s="5"/>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A198:A200" si="5">K195</f>
         <v>0</v>
       </c>
       <c r="F198" s="5"/>
@@ -5646,30 +5653,26 @@
       <c r="G202" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H202" s="2" t="str">
-        <f>IF(ISBLANK($F202)=TRUE,"",IF(ISNUMBER(FIND(H$2,VLOOKUP($F202,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v>falsch</v>
+      <c r="H202" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="I202" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J202" s="2" t="str">
-        <f>IF(ISBLANK($F202)=TRUE,"",IF(ISNUMBER(FIND(J$2,VLOOKUP($F202,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v>richtig</v>
+      <c r="J202" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="K202" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L202" s="2" t="str">
-        <f>IF(ISBLANK($F202)=TRUE,"",IF(ISNUMBER(FIND(L$2,VLOOKUP($F202,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v>richtig</v>
+      <c r="L202" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="M202" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N202" s="20" t="str">
-        <f>IF(ISBLANK($F202)=TRUE,"",IF(ISNUMBER(FIND(N$2,VLOOKUP($F202,Jimdo_Import!$C:$J,8,FALSE),1))=TRUE, "richtig", "falsch"))</f>
-        <v>falsch</v>
+      <c r="N202" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -5678,12 +5681,12 @@
       <formula1>"richtig,falsch"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Bitte wählen Sie aus, ob die Frage richtig oder falsch ist " sqref="H2:H3 H201 H203:H1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Bitte wählen Sie  ja oder nein aus." promptTitle="ja" sqref="E9:E1048576 E1:E4 E6:E7"/>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Die maximale Zeichenlänge der Antwort beträgt 55 Zeichen._x000a_Bitte kürzen Sie ihre Antwort." sqref="G9:G1048576 I9:I1048576 M9:M1048576 K9:K1048576 K4 K6:K7 M4 M6:M7 I4 I6:I7 G4 G6:G7">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Bitte wählen Sie  ja oder nein aus." promptTitle="ja" sqref="E8:E1048576 E1:E4 E5:E6"/>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Die maximale Zeichenlänge der Antwort beträgt 55 Zeichen._x000a_Bitte kürzen Sie ihre Antwort." sqref="G8:G1048576 I8:I1048576 M8:M1048576 K8:K1048576 K4 K5:K6 M4 M5:M6 I4 I5:I6 G4 G5:G6">
       <formula1>0</formula1>
       <formula2>55</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Die maximale Zeichenlänge der Frage beträgt 170 Zeichen._x000a_Bitte kürzen Sie ihre Frage." sqref="F6:F1048576 F4">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Fehler" error="Die maximale Zeichenlänge der Frage beträgt 170 Zeichen._x000a_Bitte kürzen Sie ihre Frage." sqref="F5:F1048576 F4">
       <formula1>0</formula1>
       <formula2>170</formula2>
     </dataValidation>
@@ -5749,13 +5752,13 @@
           <x14:formula1>
             <xm:f>Settings!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H4 H202 H6:H200</xm:sqref>
+          <xm:sqref>H4 H202 H5:H200</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L200 N6:N200 N4 J4 L4 N202 L202 J202 J6:J200</xm:sqref>
+          <xm:sqref>L5:L200 N5:N200 N4 J4 L4 N202 L202 J202 J5:J200</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5786,7 +5789,7 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="e">
+      <c r="C1" s="23" t="e">
         <f>A1&amp;A2&amp;A3&amp;A4&amp;A5&amp;A6&amp;A7&amp;A8&amp;A9&amp;A10&amp;A11&amp;A12&amp;A13&amp;A14&amp;A15&amp;A16&amp;A17&amp;A18&amp;A19&amp;A20&amp;A21&amp;A22&amp;A23&amp;A24&amp;A25&amp;A26&amp;A27&amp;A28&amp;A29&amp;A30&amp;A31&amp;A32&amp;A33&amp;A34&amp;A35&amp;A36&amp;A37&amp;A38&amp;A39&amp;A40&amp;A41&amp;A42&amp;A43&amp;A44&amp;A45&amp;A46&amp;A47&amp;A48&amp;A49&amp;A50</f>
         <v>#REF!</v>
       </c>
@@ -5796,841 +5799,841 @@
         <f>IF(ISBLANK(FragenTemplate!#REF!),"",("('"&amp;FragenTemplate!#REF!&amp;"', "&amp;IF(ISBLANK(FragenTemplate!#REF!),"","'"&amp;FragenTemplate!#REF!&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', "&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;",true)"&amp;IF(A3="",";",",")))</f>
         <v>#REF!</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
         <f>IF(ISBLANK(FragenTemplate!#REF!),"",("('"&amp;FragenTemplate!#REF!&amp;"', "&amp;IF(ISBLANK(FragenTemplate!#REF!),"","'"&amp;FragenTemplate!#REF!&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', '"&amp;FragenTemplate!#REF!&amp;"', "&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!#REF!,"richtig"),"true","false")&amp;",true)"&amp;IF(A4="",";",",")))</f>
         <v>#REF!</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C6),"",("('"&amp;FragenTemplate!C6&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D6),"","'"&amp;FragenTemplate!D6&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E6,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F6&amp;"', '"&amp;FragenTemplate!G6&amp;"', '"&amp;FragenTemplate!I6&amp;"', '"&amp;FragenTemplate!K6&amp;"', '"&amp;FragenTemplate!M6&amp;"', "&amp;IF(EXACT(FragenTemplate!H6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N6,"richtig"),"true","false")&amp;",true)"&amp;IF(A5="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C4" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C5),"",("('"&amp;FragenTemplate!C5&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D5),"","'"&amp;FragenTemplate!D5&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E5,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F5&amp;"', '"&amp;FragenTemplate!G5&amp;"', '"&amp;FragenTemplate!I5&amp;"', '"&amp;FragenTemplate!K5&amp;"', '"&amp;FragenTemplate!M5&amp;"', "&amp;IF(EXACT(FragenTemplate!H5,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J5,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L5,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N5,"richtig"),"true","false")&amp;",true)"&amp;IF(A5="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C7),"",("('"&amp;FragenTemplate!C7&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D7),"","'"&amp;FragenTemplate!D7&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E7,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F7&amp;"', '"&amp;FragenTemplate!G7&amp;"', '"&amp;FragenTemplate!I7&amp;"', '"&amp;FragenTemplate!K7&amp;"', '"&amp;FragenTemplate!M7&amp;"', "&amp;IF(EXACT(FragenTemplate!H7,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J7,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L7,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N7,"richtig"),"true","false")&amp;",true)"&amp;IF(A6="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C5" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C6),"",("('"&amp;FragenTemplate!C6&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D6),"","'"&amp;FragenTemplate!D6&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E6,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F6&amp;"', '"&amp;FragenTemplate!G6&amp;"', '"&amp;FragenTemplate!I6&amp;"', '"&amp;FragenTemplate!K6&amp;"', '"&amp;FragenTemplate!M6&amp;"', "&amp;IF(EXACT(FragenTemplate!H6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L6,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N6,"richtig"),"true","false")&amp;",true)"&amp;IF(A6="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C5" s="23"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF(ISBLANK(FragenTemplate!C202),"",("('"&amp;FragenTemplate!C202&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D202),"","'"&amp;FragenTemplate!D202&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E202,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F202&amp;"', '"&amp;FragenTemplate!G202&amp;"', '"&amp;FragenTemplate!I202&amp;"', '"&amp;FragenTemplate!K202&amp;"', '"&amp;FragenTemplate!M202&amp;"', "&amp;IF(EXACT(FragenTemplate!H202,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J202,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L202,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N202,"richtig"),"true","false")&amp;",true)"&amp;IF(A7="",";",",")))</f>
         <v>('Allgemeine BWL', , false, 'Für was steht BWL?', 'Busy Word Long', 'Betriebwirtschaftsehre', 'Betriebwirtschaftslehre', 'Betriebwissenslehre', false,true,true,false,true);</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C9),"",("('"&amp;FragenTemplate!C9&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D9),"","'"&amp;FragenTemplate!D9&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E9,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F9&amp;"', '"&amp;FragenTemplate!G9&amp;"', '"&amp;FragenTemplate!I9&amp;"', '"&amp;FragenTemplate!K9&amp;"', '"&amp;FragenTemplate!M9&amp;"', "&amp;IF(EXACT(FragenTemplate!H9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N9,"richtig"),"true","false")&amp;",true)"&amp;IF(A8="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C7" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C8),"",("('"&amp;FragenTemplate!C8&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D8),"","'"&amp;FragenTemplate!D8&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E8,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F8&amp;"', '"&amp;FragenTemplate!G8&amp;"', '"&amp;FragenTemplate!I8&amp;"', '"&amp;FragenTemplate!K8&amp;"', '"&amp;FragenTemplate!M8&amp;"', "&amp;IF(EXACT(FragenTemplate!H8,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J8,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L8,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N8,"richtig"),"true","false")&amp;",true)"&amp;IF(A8="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C10),"",("('"&amp;FragenTemplate!C10&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D10),"","'"&amp;FragenTemplate!D10&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E10,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F10&amp;"', '"&amp;FragenTemplate!G10&amp;"', '"&amp;FragenTemplate!I10&amp;"', '"&amp;FragenTemplate!K10&amp;"', '"&amp;FragenTemplate!M10&amp;"', "&amp;IF(EXACT(FragenTemplate!H10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N10,"richtig"),"true","false")&amp;",true)"&amp;IF(A9="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C8" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C9),"",("('"&amp;FragenTemplate!C9&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D9),"","'"&amp;FragenTemplate!D9&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E9,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F9&amp;"', '"&amp;FragenTemplate!G9&amp;"', '"&amp;FragenTemplate!I9&amp;"', '"&amp;FragenTemplate!K9&amp;"', '"&amp;FragenTemplate!M9&amp;"', "&amp;IF(EXACT(FragenTemplate!H9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L9,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N9,"richtig"),"true","false")&amp;",true)"&amp;IF(A9="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C11),"",("('"&amp;FragenTemplate!C11&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D11),"","'"&amp;FragenTemplate!D11&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E11,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F11&amp;"', '"&amp;FragenTemplate!G11&amp;"', '"&amp;FragenTemplate!I11&amp;"', '"&amp;FragenTemplate!K11&amp;"', '"&amp;FragenTemplate!M11&amp;"', "&amp;IF(EXACT(FragenTemplate!H11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N11,"richtig"),"true","false")&amp;",true)"&amp;IF(A10="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C9" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C10),"",("('"&amp;FragenTemplate!C10&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D10),"","'"&amp;FragenTemplate!D10&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E10,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F10&amp;"', '"&amp;FragenTemplate!G10&amp;"', '"&amp;FragenTemplate!I10&amp;"', '"&amp;FragenTemplate!K10&amp;"', '"&amp;FragenTemplate!M10&amp;"', "&amp;IF(EXACT(FragenTemplate!H10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L10,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N10,"richtig"),"true","false")&amp;",true)"&amp;IF(A10="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C12),"",("('"&amp;FragenTemplate!C12&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D12),"","'"&amp;FragenTemplate!D12&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E12,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F12&amp;"', '"&amp;FragenTemplate!G12&amp;"', '"&amp;FragenTemplate!I12&amp;"', '"&amp;FragenTemplate!K12&amp;"', '"&amp;FragenTemplate!M12&amp;"', "&amp;IF(EXACT(FragenTemplate!H12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N12,"richtig"),"true","false")&amp;",true)"&amp;IF(A11="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C10" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C11),"",("('"&amp;FragenTemplate!C11&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D11),"","'"&amp;FragenTemplate!D11&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E11,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F11&amp;"', '"&amp;FragenTemplate!G11&amp;"', '"&amp;FragenTemplate!I11&amp;"', '"&amp;FragenTemplate!K11&amp;"', '"&amp;FragenTemplate!M11&amp;"', "&amp;IF(EXACT(FragenTemplate!H11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L11,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N11,"richtig"),"true","false")&amp;",true)"&amp;IF(A11="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C13),"",("('"&amp;FragenTemplate!C13&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D13),"","'"&amp;FragenTemplate!D13&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E13,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F13&amp;"', '"&amp;FragenTemplate!G13&amp;"', '"&amp;FragenTemplate!I13&amp;"', '"&amp;FragenTemplate!K13&amp;"', '"&amp;FragenTemplate!M13&amp;"', "&amp;IF(EXACT(FragenTemplate!H13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N13,"richtig"),"true","false")&amp;",true)"&amp;IF(A12="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C11" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C12),"",("('"&amp;FragenTemplate!C12&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D12),"","'"&amp;FragenTemplate!D12&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E12,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F12&amp;"', '"&amp;FragenTemplate!G12&amp;"', '"&amp;FragenTemplate!I12&amp;"', '"&amp;FragenTemplate!K12&amp;"', '"&amp;FragenTemplate!M12&amp;"', "&amp;IF(EXACT(FragenTemplate!H12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L12,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N12,"richtig"),"true","false")&amp;",true)"&amp;IF(A12="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C14),"",("('"&amp;FragenTemplate!C14&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D14),"","'"&amp;FragenTemplate!D14&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E14,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F14&amp;"', '"&amp;FragenTemplate!G14&amp;"', '"&amp;FragenTemplate!I14&amp;"', '"&amp;FragenTemplate!K14&amp;"', '"&amp;FragenTemplate!M14&amp;"', "&amp;IF(EXACT(FragenTemplate!H14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N14,"richtig"),"true","false")&amp;",true)"&amp;IF(A13="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C12" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C13),"",("('"&amp;FragenTemplate!C13&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D13),"","'"&amp;FragenTemplate!D13&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E13,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F13&amp;"', '"&amp;FragenTemplate!G13&amp;"', '"&amp;FragenTemplate!I13&amp;"', '"&amp;FragenTemplate!K13&amp;"', '"&amp;FragenTemplate!M13&amp;"', "&amp;IF(EXACT(FragenTemplate!H13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L13,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N13,"richtig"),"true","false")&amp;",true)"&amp;IF(A13="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C15),"",("('"&amp;FragenTemplate!C15&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D15),"","'"&amp;FragenTemplate!D15&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E15,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F15&amp;"', '"&amp;FragenTemplate!G15&amp;"', '"&amp;FragenTemplate!I15&amp;"', '"&amp;FragenTemplate!K15&amp;"', '"&amp;FragenTemplate!M15&amp;"', "&amp;IF(EXACT(FragenTemplate!H15,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J15,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L15,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N15,"richtig"),"true","false")&amp;",true)"&amp;IF(A14="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C13" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C14),"",("('"&amp;FragenTemplate!C14&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D14),"","'"&amp;FragenTemplate!D14&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E14,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F14&amp;"', '"&amp;FragenTemplate!G14&amp;"', '"&amp;FragenTemplate!I14&amp;"', '"&amp;FragenTemplate!K14&amp;"', '"&amp;FragenTemplate!M14&amp;"', "&amp;IF(EXACT(FragenTemplate!H14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L14,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N14,"richtig"),"true","false")&amp;",true)"&amp;IF(A14="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="6"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C17),"",("('"&amp;FragenTemplate!C17&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D17),"","'"&amp;FragenTemplate!D17&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E17,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F17&amp;"', '"&amp;FragenTemplate!G17&amp;"', '"&amp;FragenTemplate!I17&amp;"', '"&amp;FragenTemplate!K17&amp;"', '"&amp;FragenTemplate!M17&amp;"', "&amp;IF(EXACT(FragenTemplate!H17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N17,"richtig"),"true","false")&amp;",true)"&amp;IF(A16="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C15" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C16),"",("('"&amp;FragenTemplate!C16&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D16),"","'"&amp;FragenTemplate!D16&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E16,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F16&amp;"', '"&amp;FragenTemplate!G16&amp;"', '"&amp;FragenTemplate!I16&amp;"', '"&amp;FragenTemplate!K16&amp;"', '"&amp;FragenTemplate!M16&amp;"', "&amp;IF(EXACT(FragenTemplate!H16,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J16,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L16,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N16,"richtig"),"true","false")&amp;",true)"&amp;IF(A16="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C18),"",("('"&amp;FragenTemplate!C18&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D18),"","'"&amp;FragenTemplate!D18&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E18,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F18&amp;"', '"&amp;FragenTemplate!G18&amp;"', '"&amp;FragenTemplate!I18&amp;"', '"&amp;FragenTemplate!K18&amp;"', '"&amp;FragenTemplate!M18&amp;"', "&amp;IF(EXACT(FragenTemplate!H18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N18,"richtig"),"true","false")&amp;",true)"&amp;IF(A17="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C16" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C17),"",("('"&amp;FragenTemplate!C17&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D17),"","'"&amp;FragenTemplate!D17&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E17,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F17&amp;"', '"&amp;FragenTemplate!G17&amp;"', '"&amp;FragenTemplate!I17&amp;"', '"&amp;FragenTemplate!K17&amp;"', '"&amp;FragenTemplate!M17&amp;"', "&amp;IF(EXACT(FragenTemplate!H17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L17,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N17,"richtig"),"true","false")&amp;",true)"&amp;IF(A17="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C19),"",("('"&amp;FragenTemplate!C19&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D19),"","'"&amp;FragenTemplate!D19&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E19,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F19&amp;"', '"&amp;FragenTemplate!G19&amp;"', '"&amp;FragenTemplate!I19&amp;"', '"&amp;FragenTemplate!K19&amp;"', '"&amp;FragenTemplate!M19&amp;"', "&amp;IF(EXACT(FragenTemplate!H19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N19,"richtig"),"true","false")&amp;",true)"&amp;IF(A18="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C17" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C18),"",("('"&amp;FragenTemplate!C18&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D18),"","'"&amp;FragenTemplate!D18&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E18,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F18&amp;"', '"&amp;FragenTemplate!G18&amp;"', '"&amp;FragenTemplate!I18&amp;"', '"&amp;FragenTemplate!K18&amp;"', '"&amp;FragenTemplate!M18&amp;"', "&amp;IF(EXACT(FragenTemplate!H18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L18,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N18,"richtig"),"true","false")&amp;",true)"&amp;IF(A18="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C20),"",("('"&amp;FragenTemplate!C20&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D20),"","'"&amp;FragenTemplate!D20&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E20,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F20&amp;"', '"&amp;FragenTemplate!G20&amp;"', '"&amp;FragenTemplate!I20&amp;"', '"&amp;FragenTemplate!K20&amp;"', '"&amp;FragenTemplate!M20&amp;"', "&amp;IF(EXACT(FragenTemplate!H20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N20,"richtig"),"true","false")&amp;",true)"&amp;IF(A19="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C18" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C19),"",("('"&amp;FragenTemplate!C19&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D19),"","'"&amp;FragenTemplate!D19&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E19,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F19&amp;"', '"&amp;FragenTemplate!G19&amp;"', '"&amp;FragenTemplate!I19&amp;"', '"&amp;FragenTemplate!K19&amp;"', '"&amp;FragenTemplate!M19&amp;"', "&amp;IF(EXACT(FragenTemplate!H19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L19,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N19,"richtig"),"true","false")&amp;",true)"&amp;IF(A19="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C21),"",("('"&amp;FragenTemplate!C21&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D21),"","'"&amp;FragenTemplate!D21&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E21,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F21&amp;"', '"&amp;FragenTemplate!G21&amp;"', '"&amp;FragenTemplate!I21&amp;"', '"&amp;FragenTemplate!K21&amp;"', '"&amp;FragenTemplate!M21&amp;"', "&amp;IF(EXACT(FragenTemplate!H21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N21,"richtig"),"true","false")&amp;",true)"&amp;IF(A20="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C19" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C20),"",("('"&amp;FragenTemplate!C20&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D20),"","'"&amp;FragenTemplate!D20&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E20,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F20&amp;"', '"&amp;FragenTemplate!G20&amp;"', '"&amp;FragenTemplate!I20&amp;"', '"&amp;FragenTemplate!K20&amp;"', '"&amp;FragenTemplate!M20&amp;"', "&amp;IF(EXACT(FragenTemplate!H20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L20,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N20,"richtig"),"true","false")&amp;",true)"&amp;IF(A20="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C22),"",("('"&amp;FragenTemplate!C22&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D22),"","'"&amp;FragenTemplate!D22&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E22,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F22&amp;"', '"&amp;FragenTemplate!G22&amp;"', '"&amp;FragenTemplate!I22&amp;"', '"&amp;FragenTemplate!K22&amp;"', '"&amp;FragenTemplate!M22&amp;"', "&amp;IF(EXACT(FragenTemplate!H22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N22,"richtig"),"true","false")&amp;",true)"&amp;IF(A21="",";",",")))</f>
-        <v/>
-      </c>
-      <c r="C20" s="6"/>
+        <f>IF(ISBLANK(FragenTemplate!C21),"",("('"&amp;FragenTemplate!C21&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D21),"","'"&amp;FragenTemplate!D21&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E21,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F21&amp;"', '"&amp;FragenTemplate!G21&amp;"', '"&amp;FragenTemplate!I21&amp;"', '"&amp;FragenTemplate!K21&amp;"', '"&amp;FragenTemplate!M21&amp;"', "&amp;IF(EXACT(FragenTemplate!H21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L21,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N21,"richtig"),"true","false")&amp;",true)"&amp;IF(A21="",";",",")))</f>
+        <v/>
+      </c>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C23),"",("('"&amp;FragenTemplate!C23&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D23),"","'"&amp;FragenTemplate!D23&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E23,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F23&amp;"', '"&amp;FragenTemplate!G23&amp;"', '"&amp;FragenTemplate!I23&amp;"', '"&amp;FragenTemplate!K23&amp;"', '"&amp;FragenTemplate!M23&amp;"', "&amp;IF(EXACT(FragenTemplate!H23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N23,"richtig"),"true","false")&amp;",true)"&amp;IF(A22="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C22),"",("('"&amp;FragenTemplate!C22&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D22),"","'"&amp;FragenTemplate!D22&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E22,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F22&amp;"', '"&amp;FragenTemplate!G22&amp;"', '"&amp;FragenTemplate!I22&amp;"', '"&amp;FragenTemplate!K22&amp;"', '"&amp;FragenTemplate!M22&amp;"', "&amp;IF(EXACT(FragenTemplate!H22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L22,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N22,"richtig"),"true","false")&amp;",true)"&amp;IF(A22="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C24),"",("('"&amp;FragenTemplate!C24&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D24),"","'"&amp;FragenTemplate!D24&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E24,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F24&amp;"', '"&amp;FragenTemplate!G24&amp;"', '"&amp;FragenTemplate!I24&amp;"', '"&amp;FragenTemplate!K24&amp;"', '"&amp;FragenTemplate!M24&amp;"', "&amp;IF(EXACT(FragenTemplate!H24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N24,"richtig"),"true","false")&amp;",true)"&amp;IF(A23="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C23),"",("('"&amp;FragenTemplate!C23&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D23),"","'"&amp;FragenTemplate!D23&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E23,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F23&amp;"', '"&amp;FragenTemplate!G23&amp;"', '"&amp;FragenTemplate!I23&amp;"', '"&amp;FragenTemplate!K23&amp;"', '"&amp;FragenTemplate!M23&amp;"', "&amp;IF(EXACT(FragenTemplate!H23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L23,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N23,"richtig"),"true","false")&amp;",true)"&amp;IF(A23="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C25),"",("('"&amp;FragenTemplate!C25&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D25),"","'"&amp;FragenTemplate!D25&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E25,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F25&amp;"', '"&amp;FragenTemplate!G25&amp;"', '"&amp;FragenTemplate!I25&amp;"', '"&amp;FragenTemplate!K25&amp;"', '"&amp;FragenTemplate!M25&amp;"', "&amp;IF(EXACT(FragenTemplate!H25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N25,"richtig"),"true","false")&amp;",true)"&amp;IF(A24="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C24),"",("('"&amp;FragenTemplate!C24&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D24),"","'"&amp;FragenTemplate!D24&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E24,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F24&amp;"', '"&amp;FragenTemplate!G24&amp;"', '"&amp;FragenTemplate!I24&amp;"', '"&amp;FragenTemplate!K24&amp;"', '"&amp;FragenTemplate!M24&amp;"', "&amp;IF(EXACT(FragenTemplate!H24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L24,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N24,"richtig"),"true","false")&amp;",true)"&amp;IF(A24="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C26),"",("('"&amp;FragenTemplate!C26&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D26),"","'"&amp;FragenTemplate!D26&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E26,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F26&amp;"', '"&amp;FragenTemplate!G26&amp;"', '"&amp;FragenTemplate!I26&amp;"', '"&amp;FragenTemplate!K26&amp;"', '"&amp;FragenTemplate!M26&amp;"', "&amp;IF(EXACT(FragenTemplate!H26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N26,"richtig"),"true","false")&amp;",true)"&amp;IF(A25="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C25),"",("('"&amp;FragenTemplate!C25&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D25),"","'"&amp;FragenTemplate!D25&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E25,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F25&amp;"', '"&amp;FragenTemplate!G25&amp;"', '"&amp;FragenTemplate!I25&amp;"', '"&amp;FragenTemplate!K25&amp;"', '"&amp;FragenTemplate!M25&amp;"', "&amp;IF(EXACT(FragenTemplate!H25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L25,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N25,"richtig"),"true","false")&amp;",true)"&amp;IF(A25="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C27),"",("('"&amp;FragenTemplate!C27&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D27),"","'"&amp;FragenTemplate!D27&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E27,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F27&amp;"', '"&amp;FragenTemplate!G27&amp;"', '"&amp;FragenTemplate!I27&amp;"', '"&amp;FragenTemplate!K27&amp;"', '"&amp;FragenTemplate!M27&amp;"', "&amp;IF(EXACT(FragenTemplate!H27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N27,"richtig"),"true","false")&amp;",true)"&amp;IF(A26="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C26),"",("('"&amp;FragenTemplate!C26&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D26),"","'"&amp;FragenTemplate!D26&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E26,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F26&amp;"', '"&amp;FragenTemplate!G26&amp;"', '"&amp;FragenTemplate!I26&amp;"', '"&amp;FragenTemplate!K26&amp;"', '"&amp;FragenTemplate!M26&amp;"', "&amp;IF(EXACT(FragenTemplate!H26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L26,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N26,"richtig"),"true","false")&amp;",true)"&amp;IF(A26="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C28),"",("('"&amp;FragenTemplate!C28&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D28),"","'"&amp;FragenTemplate!D28&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E28,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F28&amp;"', '"&amp;FragenTemplate!G28&amp;"', '"&amp;FragenTemplate!I28&amp;"', '"&amp;FragenTemplate!K28&amp;"', '"&amp;FragenTemplate!M28&amp;"', "&amp;IF(EXACT(FragenTemplate!H28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N28,"richtig"),"true","false")&amp;",true)"&amp;IF(A27="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C27),"",("('"&amp;FragenTemplate!C27&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D27),"","'"&amp;FragenTemplate!D27&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E27,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F27&amp;"', '"&amp;FragenTemplate!G27&amp;"', '"&amp;FragenTemplate!I27&amp;"', '"&amp;FragenTemplate!K27&amp;"', '"&amp;FragenTemplate!M27&amp;"', "&amp;IF(EXACT(FragenTemplate!H27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L27,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N27,"richtig"),"true","false")&amp;",true)"&amp;IF(A27="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C29),"",("('"&amp;FragenTemplate!C29&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D29),"","'"&amp;FragenTemplate!D29&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E29,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F29&amp;"', '"&amp;FragenTemplate!G29&amp;"', '"&amp;FragenTemplate!I29&amp;"', '"&amp;FragenTemplate!K29&amp;"', '"&amp;FragenTemplate!M29&amp;"', "&amp;IF(EXACT(FragenTemplate!H29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N29,"richtig"),"true","false")&amp;",true)"&amp;IF(A28="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C28),"",("('"&amp;FragenTemplate!C28&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D28),"","'"&amp;FragenTemplate!D28&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E28,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F28&amp;"', '"&amp;FragenTemplate!G28&amp;"', '"&amp;FragenTemplate!I28&amp;"', '"&amp;FragenTemplate!K28&amp;"', '"&amp;FragenTemplate!M28&amp;"', "&amp;IF(EXACT(FragenTemplate!H28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L28,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N28,"richtig"),"true","false")&amp;",true)"&amp;IF(A28="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C30),"",("('"&amp;FragenTemplate!C30&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D30),"","'"&amp;FragenTemplate!D30&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E30,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F30&amp;"', '"&amp;FragenTemplate!G30&amp;"', '"&amp;FragenTemplate!I30&amp;"', '"&amp;FragenTemplate!K30&amp;"', '"&amp;FragenTemplate!M30&amp;"', "&amp;IF(EXACT(FragenTemplate!H30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N30,"richtig"),"true","false")&amp;",true)"&amp;IF(A29="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C29),"",("('"&amp;FragenTemplate!C29&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D29),"","'"&amp;FragenTemplate!D29&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E29,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F29&amp;"', '"&amp;FragenTemplate!G29&amp;"', '"&amp;FragenTemplate!I29&amp;"', '"&amp;FragenTemplate!K29&amp;"', '"&amp;FragenTemplate!M29&amp;"', "&amp;IF(EXACT(FragenTemplate!H29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L29,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N29,"richtig"),"true","false")&amp;",true)"&amp;IF(A29="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C31),"",("('"&amp;FragenTemplate!C31&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D31),"","'"&amp;FragenTemplate!D31&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E31,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F31&amp;"', '"&amp;FragenTemplate!G31&amp;"', '"&amp;FragenTemplate!I31&amp;"', '"&amp;FragenTemplate!K31&amp;"', '"&amp;FragenTemplate!M31&amp;"', "&amp;IF(EXACT(FragenTemplate!H31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N31,"richtig"),"true","false")&amp;",true)"&amp;IF(A30="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C30),"",("('"&amp;FragenTemplate!C30&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D30),"","'"&amp;FragenTemplate!D30&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E30,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F30&amp;"', '"&amp;FragenTemplate!G30&amp;"', '"&amp;FragenTemplate!I30&amp;"', '"&amp;FragenTemplate!K30&amp;"', '"&amp;FragenTemplate!M30&amp;"', "&amp;IF(EXACT(FragenTemplate!H30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L30,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N30,"richtig"),"true","false")&amp;",true)"&amp;IF(A30="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C32),"",("('"&amp;FragenTemplate!C32&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D32),"","'"&amp;FragenTemplate!D32&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E32,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F32&amp;"', '"&amp;FragenTemplate!G32&amp;"', '"&amp;FragenTemplate!I32&amp;"', '"&amp;FragenTemplate!K32&amp;"', '"&amp;FragenTemplate!M32&amp;"', "&amp;IF(EXACT(FragenTemplate!H32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N32,"richtig"),"true","false")&amp;",true)"&amp;IF(A31="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C31),"",("('"&amp;FragenTemplate!C31&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D31),"","'"&amp;FragenTemplate!D31&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E31,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F31&amp;"', '"&amp;FragenTemplate!G31&amp;"', '"&amp;FragenTemplate!I31&amp;"', '"&amp;FragenTemplate!K31&amp;"', '"&amp;FragenTemplate!M31&amp;"', "&amp;IF(EXACT(FragenTemplate!H31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L31,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N31,"richtig"),"true","false")&amp;",true)"&amp;IF(A31="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C33),"",("('"&amp;FragenTemplate!C33&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D33),"","'"&amp;FragenTemplate!D33&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E33,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F33&amp;"', '"&amp;FragenTemplate!G33&amp;"', '"&amp;FragenTemplate!I33&amp;"', '"&amp;FragenTemplate!K33&amp;"', '"&amp;FragenTemplate!M33&amp;"', "&amp;IF(EXACT(FragenTemplate!H33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N33,"richtig"),"true","false")&amp;",true)"&amp;IF(A32="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C32),"",("('"&amp;FragenTemplate!C32&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D32),"","'"&amp;FragenTemplate!D32&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E32,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F32&amp;"', '"&amp;FragenTemplate!G32&amp;"', '"&amp;FragenTemplate!I32&amp;"', '"&amp;FragenTemplate!K32&amp;"', '"&amp;FragenTemplate!M32&amp;"', "&amp;IF(EXACT(FragenTemplate!H32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L32,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N32,"richtig"),"true","false")&amp;",true)"&amp;IF(A32="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C34),"",("('"&amp;FragenTemplate!C34&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D34),"","'"&amp;FragenTemplate!D34&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E34,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F34&amp;"', '"&amp;FragenTemplate!G34&amp;"', '"&amp;FragenTemplate!I34&amp;"', '"&amp;FragenTemplate!K34&amp;"', '"&amp;FragenTemplate!M34&amp;"', "&amp;IF(EXACT(FragenTemplate!H34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N34,"richtig"),"true","false")&amp;",true)"&amp;IF(A33="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C33),"",("('"&amp;FragenTemplate!C33&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D33),"","'"&amp;FragenTemplate!D33&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E33,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F33&amp;"', '"&amp;FragenTemplate!G33&amp;"', '"&amp;FragenTemplate!I33&amp;"', '"&amp;FragenTemplate!K33&amp;"', '"&amp;FragenTemplate!M33&amp;"', "&amp;IF(EXACT(FragenTemplate!H33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L33,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N33,"richtig"),"true","false")&amp;",true)"&amp;IF(A33="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C35),"",("('"&amp;FragenTemplate!C35&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D35),"","'"&amp;FragenTemplate!D35&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E35,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F35&amp;"', '"&amp;FragenTemplate!G35&amp;"', '"&amp;FragenTemplate!I35&amp;"', '"&amp;FragenTemplate!K35&amp;"', '"&amp;FragenTemplate!M35&amp;"', "&amp;IF(EXACT(FragenTemplate!H35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N35,"richtig"),"true","false")&amp;",true)"&amp;IF(A34="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C34),"",("('"&amp;FragenTemplate!C34&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D34),"","'"&amp;FragenTemplate!D34&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E34,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F34&amp;"', '"&amp;FragenTemplate!G34&amp;"', '"&amp;FragenTemplate!I34&amp;"', '"&amp;FragenTemplate!K34&amp;"', '"&amp;FragenTemplate!M34&amp;"', "&amp;IF(EXACT(FragenTemplate!H34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L34,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N34,"richtig"),"true","false")&amp;",true)"&amp;IF(A34="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C36),"",("('"&amp;FragenTemplate!C36&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D36),"","'"&amp;FragenTemplate!D36&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E36,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F36&amp;"', '"&amp;FragenTemplate!G36&amp;"', '"&amp;FragenTemplate!I36&amp;"', '"&amp;FragenTemplate!K36&amp;"', '"&amp;FragenTemplate!M36&amp;"', "&amp;IF(EXACT(FragenTemplate!H36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N36,"richtig"),"true","false")&amp;",true)"&amp;IF(A35="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C35),"",("('"&amp;FragenTemplate!C35&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D35),"","'"&amp;FragenTemplate!D35&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E35,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F35&amp;"', '"&amp;FragenTemplate!G35&amp;"', '"&amp;FragenTemplate!I35&amp;"', '"&amp;FragenTemplate!K35&amp;"', '"&amp;FragenTemplate!M35&amp;"', "&amp;IF(EXACT(FragenTemplate!H35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L35,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N35,"richtig"),"true","false")&amp;",true)"&amp;IF(A35="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C37),"",("('"&amp;FragenTemplate!C37&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D37),"","'"&amp;FragenTemplate!D37&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E37,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F37&amp;"', '"&amp;FragenTemplate!G37&amp;"', '"&amp;FragenTemplate!I37&amp;"', '"&amp;FragenTemplate!K37&amp;"', '"&amp;FragenTemplate!M37&amp;"', "&amp;IF(EXACT(FragenTemplate!H37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N37,"richtig"),"true","false")&amp;",true)"&amp;IF(A36="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C36),"",("('"&amp;FragenTemplate!C36&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D36),"","'"&amp;FragenTemplate!D36&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E36,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F36&amp;"', '"&amp;FragenTemplate!G36&amp;"', '"&amp;FragenTemplate!I36&amp;"', '"&amp;FragenTemplate!K36&amp;"', '"&amp;FragenTemplate!M36&amp;"', "&amp;IF(EXACT(FragenTemplate!H36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L36,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N36,"richtig"),"true","false")&amp;",true)"&amp;IF(A36="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C38),"",("('"&amp;FragenTemplate!C38&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D38),"","'"&amp;FragenTemplate!D38&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E38,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F38&amp;"', '"&amp;FragenTemplate!G38&amp;"', '"&amp;FragenTemplate!I38&amp;"', '"&amp;FragenTemplate!K38&amp;"', '"&amp;FragenTemplate!M38&amp;"', "&amp;IF(EXACT(FragenTemplate!H38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N38,"richtig"),"true","false")&amp;",true)"&amp;IF(A37="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C37),"",("('"&amp;FragenTemplate!C37&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D37),"","'"&amp;FragenTemplate!D37&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E37,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F37&amp;"', '"&amp;FragenTemplate!G37&amp;"', '"&amp;FragenTemplate!I37&amp;"', '"&amp;FragenTemplate!K37&amp;"', '"&amp;FragenTemplate!M37&amp;"', "&amp;IF(EXACT(FragenTemplate!H37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L37,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N37,"richtig"),"true","false")&amp;",true)"&amp;IF(A37="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C39),"",("('"&amp;FragenTemplate!C39&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D39),"","'"&amp;FragenTemplate!D39&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E39,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F39&amp;"', '"&amp;FragenTemplate!G39&amp;"', '"&amp;FragenTemplate!I39&amp;"', '"&amp;FragenTemplate!K39&amp;"', '"&amp;FragenTemplate!M39&amp;"', "&amp;IF(EXACT(FragenTemplate!H39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N39,"richtig"),"true","false")&amp;",true)"&amp;IF(A38="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C38),"",("('"&amp;FragenTemplate!C38&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D38),"","'"&amp;FragenTemplate!D38&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E38,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F38&amp;"', '"&amp;FragenTemplate!G38&amp;"', '"&amp;FragenTemplate!I38&amp;"', '"&amp;FragenTemplate!K38&amp;"', '"&amp;FragenTemplate!M38&amp;"', "&amp;IF(EXACT(FragenTemplate!H38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L38,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N38,"richtig"),"true","false")&amp;",true)"&amp;IF(A38="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C40),"",("('"&amp;FragenTemplate!C40&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D40),"","'"&amp;FragenTemplate!D40&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E40,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F40&amp;"', '"&amp;FragenTemplate!G40&amp;"', '"&amp;FragenTemplate!I40&amp;"', '"&amp;FragenTemplate!K40&amp;"', '"&amp;FragenTemplate!M40&amp;"', "&amp;IF(EXACT(FragenTemplate!H40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N40,"richtig"),"true","false")&amp;",true)"&amp;IF(A39="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C39),"",("('"&amp;FragenTemplate!C39&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D39),"","'"&amp;FragenTemplate!D39&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E39,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F39&amp;"', '"&amp;FragenTemplate!G39&amp;"', '"&amp;FragenTemplate!I39&amp;"', '"&amp;FragenTemplate!K39&amp;"', '"&amp;FragenTemplate!M39&amp;"', "&amp;IF(EXACT(FragenTemplate!H39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L39,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N39,"richtig"),"true","false")&amp;",true)"&amp;IF(A39="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C41),"",("('"&amp;FragenTemplate!C41&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D41),"","'"&amp;FragenTemplate!D41&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E41,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F41&amp;"', '"&amp;FragenTemplate!G41&amp;"', '"&amp;FragenTemplate!I41&amp;"', '"&amp;FragenTemplate!K41&amp;"', '"&amp;FragenTemplate!M41&amp;"', "&amp;IF(EXACT(FragenTemplate!H41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N41,"richtig"),"true","false")&amp;",true)"&amp;IF(A40="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C40),"",("('"&amp;FragenTemplate!C40&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D40),"","'"&amp;FragenTemplate!D40&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E40,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F40&amp;"', '"&amp;FragenTemplate!G40&amp;"', '"&amp;FragenTemplate!I40&amp;"', '"&amp;FragenTemplate!K40&amp;"', '"&amp;FragenTemplate!M40&amp;"', "&amp;IF(EXACT(FragenTemplate!H40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L40,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N40,"richtig"),"true","false")&amp;",true)"&amp;IF(A40="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C42),"",("('"&amp;FragenTemplate!C42&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D42),"","'"&amp;FragenTemplate!D42&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E42,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F42&amp;"', '"&amp;FragenTemplate!G42&amp;"', '"&amp;FragenTemplate!I42&amp;"', '"&amp;FragenTemplate!K42&amp;"', '"&amp;FragenTemplate!M42&amp;"', "&amp;IF(EXACT(FragenTemplate!H42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N42,"richtig"),"true","false")&amp;",true)"&amp;IF(A41="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C41),"",("('"&amp;FragenTemplate!C41&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D41),"","'"&amp;FragenTemplate!D41&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E41,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F41&amp;"', '"&amp;FragenTemplate!G41&amp;"', '"&amp;FragenTemplate!I41&amp;"', '"&amp;FragenTemplate!K41&amp;"', '"&amp;FragenTemplate!M41&amp;"', "&amp;IF(EXACT(FragenTemplate!H41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L41,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N41,"richtig"),"true","false")&amp;",true)"&amp;IF(A41="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C43),"",("('"&amp;FragenTemplate!C43&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D43),"","'"&amp;FragenTemplate!D43&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E43,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F43&amp;"', '"&amp;FragenTemplate!G43&amp;"', '"&amp;FragenTemplate!I43&amp;"', '"&amp;FragenTemplate!K43&amp;"', '"&amp;FragenTemplate!M43&amp;"', "&amp;IF(EXACT(FragenTemplate!H43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N43,"richtig"),"true","false")&amp;",true)"&amp;IF(A42="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C42),"",("('"&amp;FragenTemplate!C42&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D42),"","'"&amp;FragenTemplate!D42&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E42,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F42&amp;"', '"&amp;FragenTemplate!G42&amp;"', '"&amp;FragenTemplate!I42&amp;"', '"&amp;FragenTemplate!K42&amp;"', '"&amp;FragenTemplate!M42&amp;"', "&amp;IF(EXACT(FragenTemplate!H42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L42,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N42,"richtig"),"true","false")&amp;",true)"&amp;IF(A42="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C44),"",("('"&amp;FragenTemplate!C44&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D44),"","'"&amp;FragenTemplate!D44&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E44,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F44&amp;"', '"&amp;FragenTemplate!G44&amp;"', '"&amp;FragenTemplate!I44&amp;"', '"&amp;FragenTemplate!K44&amp;"', '"&amp;FragenTemplate!M44&amp;"', "&amp;IF(EXACT(FragenTemplate!H44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N44,"richtig"),"true","false")&amp;",true)"&amp;IF(A43="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C43),"",("('"&amp;FragenTemplate!C43&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D43),"","'"&amp;FragenTemplate!D43&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E43,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F43&amp;"', '"&amp;FragenTemplate!G43&amp;"', '"&amp;FragenTemplate!I43&amp;"', '"&amp;FragenTemplate!K43&amp;"', '"&amp;FragenTemplate!M43&amp;"', "&amp;IF(EXACT(FragenTemplate!H43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L43,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N43,"richtig"),"true","false")&amp;",true)"&amp;IF(A43="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C45),"",("('"&amp;FragenTemplate!C45&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D45),"","'"&amp;FragenTemplate!D45&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E45,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F45&amp;"', '"&amp;FragenTemplate!G45&amp;"', '"&amp;FragenTemplate!I45&amp;"', '"&amp;FragenTemplate!K45&amp;"', '"&amp;FragenTemplate!M45&amp;"', "&amp;IF(EXACT(FragenTemplate!H45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N45,"richtig"),"true","false")&amp;",true)"&amp;IF(A44="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C44),"",("('"&amp;FragenTemplate!C44&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D44),"","'"&amp;FragenTemplate!D44&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E44,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F44&amp;"', '"&amp;FragenTemplate!G44&amp;"', '"&amp;FragenTemplate!I44&amp;"', '"&amp;FragenTemplate!K44&amp;"', '"&amp;FragenTemplate!M44&amp;"', "&amp;IF(EXACT(FragenTemplate!H44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L44,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N44,"richtig"),"true","false")&amp;",true)"&amp;IF(A44="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C46),"",("('"&amp;FragenTemplate!C46&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D46),"","'"&amp;FragenTemplate!D46&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E46,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F46&amp;"', '"&amp;FragenTemplate!G46&amp;"', '"&amp;FragenTemplate!I46&amp;"', '"&amp;FragenTemplate!K46&amp;"', '"&amp;FragenTemplate!M46&amp;"', "&amp;IF(EXACT(FragenTemplate!H46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N46,"richtig"),"true","false")&amp;",true)"&amp;IF(A45="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C45),"",("('"&amp;FragenTemplate!C45&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D45),"","'"&amp;FragenTemplate!D45&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E45,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F45&amp;"', '"&amp;FragenTemplate!G45&amp;"', '"&amp;FragenTemplate!I45&amp;"', '"&amp;FragenTemplate!K45&amp;"', '"&amp;FragenTemplate!M45&amp;"', "&amp;IF(EXACT(FragenTemplate!H45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L45,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N45,"richtig"),"true","false")&amp;",true)"&amp;IF(A45="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C47),"",("('"&amp;FragenTemplate!C47&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D47),"","'"&amp;FragenTemplate!D47&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E47,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F47&amp;"', '"&amp;FragenTemplate!G47&amp;"', '"&amp;FragenTemplate!I47&amp;"', '"&amp;FragenTemplate!K47&amp;"', '"&amp;FragenTemplate!M47&amp;"', "&amp;IF(EXACT(FragenTemplate!H47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N47,"richtig"),"true","false")&amp;",true)"&amp;IF(A46="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C46),"",("('"&amp;FragenTemplate!C46&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D46),"","'"&amp;FragenTemplate!D46&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E46,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F46&amp;"', '"&amp;FragenTemplate!G46&amp;"', '"&amp;FragenTemplate!I46&amp;"', '"&amp;FragenTemplate!K46&amp;"', '"&amp;FragenTemplate!M46&amp;"', "&amp;IF(EXACT(FragenTemplate!H46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L46,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N46,"richtig"),"true","false")&amp;",true)"&amp;IF(A46="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C48),"",("('"&amp;FragenTemplate!C48&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D48),"","'"&amp;FragenTemplate!D48&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E48,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F48&amp;"', '"&amp;FragenTemplate!G48&amp;"', '"&amp;FragenTemplate!I48&amp;"', '"&amp;FragenTemplate!K48&amp;"', '"&amp;FragenTemplate!M48&amp;"', "&amp;IF(EXACT(FragenTemplate!H48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N48,"richtig"),"true","false")&amp;",true)"&amp;IF(A47="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C47),"",("('"&amp;FragenTemplate!C47&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D47),"","'"&amp;FragenTemplate!D47&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E47,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F47&amp;"', '"&amp;FragenTemplate!G47&amp;"', '"&amp;FragenTemplate!I47&amp;"', '"&amp;FragenTemplate!K47&amp;"', '"&amp;FragenTemplate!M47&amp;"', "&amp;IF(EXACT(FragenTemplate!H47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L47,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N47,"richtig"),"true","false")&amp;",true)"&amp;IF(A47="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C49),"",("('"&amp;FragenTemplate!C49&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D49),"","'"&amp;FragenTemplate!D49&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E49,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F49&amp;"', '"&amp;FragenTemplate!G49&amp;"', '"&amp;FragenTemplate!I49&amp;"', '"&amp;FragenTemplate!K49&amp;"', '"&amp;FragenTemplate!M49&amp;"', "&amp;IF(EXACT(FragenTemplate!H49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N49,"richtig"),"true","false")&amp;",true)"&amp;IF(A48="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C48),"",("('"&amp;FragenTemplate!C48&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D48),"","'"&amp;FragenTemplate!D48&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E48,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F48&amp;"', '"&amp;FragenTemplate!G48&amp;"', '"&amp;FragenTemplate!I48&amp;"', '"&amp;FragenTemplate!K48&amp;"', '"&amp;FragenTemplate!M48&amp;"', "&amp;IF(EXACT(FragenTemplate!H48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L48,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N48,"richtig"),"true","false")&amp;",true)"&amp;IF(A48="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C50),"",("('"&amp;FragenTemplate!C50&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D50),"","'"&amp;FragenTemplate!D50&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E50,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F50&amp;"', '"&amp;FragenTemplate!G50&amp;"', '"&amp;FragenTemplate!I50&amp;"', '"&amp;FragenTemplate!K50&amp;"', '"&amp;FragenTemplate!M50&amp;"', "&amp;IF(EXACT(FragenTemplate!H50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N50,"richtig"),"true","false")&amp;",true)"&amp;IF(A49="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C49),"",("('"&amp;FragenTemplate!C49&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D49),"","'"&amp;FragenTemplate!D49&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E49,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F49&amp;"', '"&amp;FragenTemplate!G49&amp;"', '"&amp;FragenTemplate!I49&amp;"', '"&amp;FragenTemplate!K49&amp;"', '"&amp;FragenTemplate!M49&amp;"', "&amp;IF(EXACT(FragenTemplate!H49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L49,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N49,"richtig"),"true","false")&amp;",true)"&amp;IF(A49="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C51),"",("('"&amp;FragenTemplate!C51&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D51),"","'"&amp;FragenTemplate!D51&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E51,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F51&amp;"', '"&amp;FragenTemplate!G51&amp;"', '"&amp;FragenTemplate!I51&amp;"', '"&amp;FragenTemplate!K51&amp;"', '"&amp;FragenTemplate!M51&amp;"', "&amp;IF(EXACT(FragenTemplate!H51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N51,"richtig"),"true","false")&amp;",true)"&amp;IF(A50="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C50),"",("('"&amp;FragenTemplate!C50&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D50),"","'"&amp;FragenTemplate!D50&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E50,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F50&amp;"', '"&amp;FragenTemplate!G50&amp;"', '"&amp;FragenTemplate!I50&amp;"', '"&amp;FragenTemplate!K50&amp;"', '"&amp;FragenTemplate!M50&amp;"', "&amp;IF(EXACT(FragenTemplate!H50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L50,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N50,"richtig"),"true","false")&amp;",true)"&amp;IF(A50="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C52),"",("('"&amp;FragenTemplate!C52&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D52),"","'"&amp;FragenTemplate!D52&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E52,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F52&amp;"', '"&amp;FragenTemplate!G52&amp;"', '"&amp;FragenTemplate!I52&amp;"', '"&amp;FragenTemplate!K52&amp;"', '"&amp;FragenTemplate!M52&amp;"', "&amp;IF(EXACT(FragenTemplate!H52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N52,"richtig"),"true","false")&amp;",true)"&amp;IF(A51="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C51),"",("('"&amp;FragenTemplate!C51&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D51),"","'"&amp;FragenTemplate!D51&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E51,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F51&amp;"', '"&amp;FragenTemplate!G51&amp;"', '"&amp;FragenTemplate!I51&amp;"', '"&amp;FragenTemplate!K51&amp;"', '"&amp;FragenTemplate!M51&amp;"', "&amp;IF(EXACT(FragenTemplate!H51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L51,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N51,"richtig"),"true","false")&amp;",true)"&amp;IF(A51="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C53),"",("('"&amp;FragenTemplate!C53&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D53),"","'"&amp;FragenTemplate!D53&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E53,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F53&amp;"', '"&amp;FragenTemplate!G53&amp;"', '"&amp;FragenTemplate!I53&amp;"', '"&amp;FragenTemplate!K53&amp;"', '"&amp;FragenTemplate!M53&amp;"', "&amp;IF(EXACT(FragenTemplate!H53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N53,"richtig"),"true","false")&amp;",true)"&amp;IF(A52="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C52),"",("('"&amp;FragenTemplate!C52&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D52),"","'"&amp;FragenTemplate!D52&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E52,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F52&amp;"', '"&amp;FragenTemplate!G52&amp;"', '"&amp;FragenTemplate!I52&amp;"', '"&amp;FragenTemplate!K52&amp;"', '"&amp;FragenTemplate!M52&amp;"', "&amp;IF(EXACT(FragenTemplate!H52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L52,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N52,"richtig"),"true","false")&amp;",true)"&amp;IF(A52="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C54),"",("('"&amp;FragenTemplate!C54&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D54),"","'"&amp;FragenTemplate!D54&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E54,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F54&amp;"', '"&amp;FragenTemplate!G54&amp;"', '"&amp;FragenTemplate!I54&amp;"', '"&amp;FragenTemplate!K54&amp;"', '"&amp;FragenTemplate!M54&amp;"', "&amp;IF(EXACT(FragenTemplate!H54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N54,"richtig"),"true","false")&amp;",true)"&amp;IF(A53="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C53),"",("('"&amp;FragenTemplate!C53&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D53),"","'"&amp;FragenTemplate!D53&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E53,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F53&amp;"', '"&amp;FragenTemplate!G53&amp;"', '"&amp;FragenTemplate!I53&amp;"', '"&amp;FragenTemplate!K53&amp;"', '"&amp;FragenTemplate!M53&amp;"', "&amp;IF(EXACT(FragenTemplate!H53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L53,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N53,"richtig"),"true","false")&amp;",true)"&amp;IF(A53="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C55),"",("('"&amp;FragenTemplate!C55&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D55),"","'"&amp;FragenTemplate!D55&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E55,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F55&amp;"', '"&amp;FragenTemplate!G55&amp;"', '"&amp;FragenTemplate!I55&amp;"', '"&amp;FragenTemplate!K55&amp;"', '"&amp;FragenTemplate!M55&amp;"', "&amp;IF(EXACT(FragenTemplate!H55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N55,"richtig"),"true","false")&amp;",true)"&amp;IF(A54="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C54),"",("('"&amp;FragenTemplate!C54&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D54),"","'"&amp;FragenTemplate!D54&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E54,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F54&amp;"', '"&amp;FragenTemplate!G54&amp;"', '"&amp;FragenTemplate!I54&amp;"', '"&amp;FragenTemplate!K54&amp;"', '"&amp;FragenTemplate!M54&amp;"', "&amp;IF(EXACT(FragenTemplate!H54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L54,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N54,"richtig"),"true","false")&amp;",true)"&amp;IF(A54="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C56),"",("('"&amp;FragenTemplate!C56&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D56),"","'"&amp;FragenTemplate!D56&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E56,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F56&amp;"', '"&amp;FragenTemplate!G56&amp;"', '"&amp;FragenTemplate!I56&amp;"', '"&amp;FragenTemplate!K56&amp;"', '"&amp;FragenTemplate!M56&amp;"', "&amp;IF(EXACT(FragenTemplate!H56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N56,"richtig"),"true","false")&amp;",true)"&amp;IF(A55="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C55),"",("('"&amp;FragenTemplate!C55&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D55),"","'"&amp;FragenTemplate!D55&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E55,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F55&amp;"', '"&amp;FragenTemplate!G55&amp;"', '"&amp;FragenTemplate!I55&amp;"', '"&amp;FragenTemplate!K55&amp;"', '"&amp;FragenTemplate!M55&amp;"', "&amp;IF(EXACT(FragenTemplate!H55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L55,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N55,"richtig"),"true","false")&amp;",true)"&amp;IF(A55="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C57),"",("('"&amp;FragenTemplate!C57&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D57),"","'"&amp;FragenTemplate!D57&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E57,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F57&amp;"', '"&amp;FragenTemplate!G57&amp;"', '"&amp;FragenTemplate!I57&amp;"', '"&amp;FragenTemplate!K57&amp;"', '"&amp;FragenTemplate!M57&amp;"', "&amp;IF(EXACT(FragenTemplate!H57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N57,"richtig"),"true","false")&amp;",true)"&amp;IF(A56="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C56),"",("('"&amp;FragenTemplate!C56&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D56),"","'"&amp;FragenTemplate!D56&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E56,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F56&amp;"', '"&amp;FragenTemplate!G56&amp;"', '"&amp;FragenTemplate!I56&amp;"', '"&amp;FragenTemplate!K56&amp;"', '"&amp;FragenTemplate!M56&amp;"', "&amp;IF(EXACT(FragenTemplate!H56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L56,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N56,"richtig"),"true","false")&amp;",true)"&amp;IF(A56="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C58),"",("('"&amp;FragenTemplate!C58&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D58),"","'"&amp;FragenTemplate!D58&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E58,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F58&amp;"', '"&amp;FragenTemplate!G58&amp;"', '"&amp;FragenTemplate!I58&amp;"', '"&amp;FragenTemplate!K58&amp;"', '"&amp;FragenTemplate!M58&amp;"', "&amp;IF(EXACT(FragenTemplate!H58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N58,"richtig"),"true","false")&amp;",true)"&amp;IF(A57="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C57),"",("('"&amp;FragenTemplate!C57&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D57),"","'"&amp;FragenTemplate!D57&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E57,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F57&amp;"', '"&amp;FragenTemplate!G57&amp;"', '"&amp;FragenTemplate!I57&amp;"', '"&amp;FragenTemplate!K57&amp;"', '"&amp;FragenTemplate!M57&amp;"', "&amp;IF(EXACT(FragenTemplate!H57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L57,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N57,"richtig"),"true","false")&amp;",true)"&amp;IF(A57="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C59),"",("('"&amp;FragenTemplate!C59&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D59),"","'"&amp;FragenTemplate!D59&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E59,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F59&amp;"', '"&amp;FragenTemplate!G59&amp;"', '"&amp;FragenTemplate!I59&amp;"', '"&amp;FragenTemplate!K59&amp;"', '"&amp;FragenTemplate!M59&amp;"', "&amp;IF(EXACT(FragenTemplate!H59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N59,"richtig"),"true","false")&amp;",true)"&amp;IF(A58="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C58),"",("('"&amp;FragenTemplate!C58&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D58),"","'"&amp;FragenTemplate!D58&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E58,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F58&amp;"', '"&amp;FragenTemplate!G58&amp;"', '"&amp;FragenTemplate!I58&amp;"', '"&amp;FragenTemplate!K58&amp;"', '"&amp;FragenTemplate!M58&amp;"', "&amp;IF(EXACT(FragenTemplate!H58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L58,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N58,"richtig"),"true","false")&amp;",true)"&amp;IF(A58="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C60),"",("('"&amp;FragenTemplate!C60&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D60),"","'"&amp;FragenTemplate!D60&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E60,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F60&amp;"', '"&amp;FragenTemplate!G60&amp;"', '"&amp;FragenTemplate!I60&amp;"', '"&amp;FragenTemplate!K60&amp;"', '"&amp;FragenTemplate!M60&amp;"', "&amp;IF(EXACT(FragenTemplate!H60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N60,"richtig"),"true","false")&amp;",true)"&amp;IF(A59="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C59),"",("('"&amp;FragenTemplate!C59&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D59),"","'"&amp;FragenTemplate!D59&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E59,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F59&amp;"', '"&amp;FragenTemplate!G59&amp;"', '"&amp;FragenTemplate!I59&amp;"', '"&amp;FragenTemplate!K59&amp;"', '"&amp;FragenTemplate!M59&amp;"', "&amp;IF(EXACT(FragenTemplate!H59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L59,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N59,"richtig"),"true","false")&amp;",true)"&amp;IF(A59="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C61),"",("('"&amp;FragenTemplate!C61&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D61),"","'"&amp;FragenTemplate!D61&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E61,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F61&amp;"', '"&amp;FragenTemplate!G61&amp;"', '"&amp;FragenTemplate!I61&amp;"', '"&amp;FragenTemplate!K61&amp;"', '"&amp;FragenTemplate!M61&amp;"', "&amp;IF(EXACT(FragenTemplate!H61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N61,"richtig"),"true","false")&amp;",true)"&amp;IF(A60="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C60),"",("('"&amp;FragenTemplate!C60&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D60),"","'"&amp;FragenTemplate!D60&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E60,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F60&amp;"', '"&amp;FragenTemplate!G60&amp;"', '"&amp;FragenTemplate!I60&amp;"', '"&amp;FragenTemplate!K60&amp;"', '"&amp;FragenTemplate!M60&amp;"', "&amp;IF(EXACT(FragenTemplate!H60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L60,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N60,"richtig"),"true","false")&amp;",true)"&amp;IF(A60="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C62),"",("('"&amp;FragenTemplate!C62&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D62),"","'"&amp;FragenTemplate!D62&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E62,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F62&amp;"', '"&amp;FragenTemplate!G62&amp;"', '"&amp;FragenTemplate!I62&amp;"', '"&amp;FragenTemplate!K62&amp;"', '"&amp;FragenTemplate!M62&amp;"', "&amp;IF(EXACT(FragenTemplate!H62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N62,"richtig"),"true","false")&amp;",true)"&amp;IF(A61="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C61),"",("('"&amp;FragenTemplate!C61&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D61),"","'"&amp;FragenTemplate!D61&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E61,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F61&amp;"', '"&amp;FragenTemplate!G61&amp;"', '"&amp;FragenTemplate!I61&amp;"', '"&amp;FragenTemplate!K61&amp;"', '"&amp;FragenTemplate!M61&amp;"', "&amp;IF(EXACT(FragenTemplate!H61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L61,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N61,"richtig"),"true","false")&amp;",true)"&amp;IF(A61="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C63),"",("('"&amp;FragenTemplate!C63&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D63),"","'"&amp;FragenTemplate!D63&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E63,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F63&amp;"', '"&amp;FragenTemplate!G63&amp;"', '"&amp;FragenTemplate!I63&amp;"', '"&amp;FragenTemplate!K63&amp;"', '"&amp;FragenTemplate!M63&amp;"', "&amp;IF(EXACT(FragenTemplate!H63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N63,"richtig"),"true","false")&amp;",true)"&amp;IF(A62="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C62),"",("('"&amp;FragenTemplate!C62&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D62),"","'"&amp;FragenTemplate!D62&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E62,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F62&amp;"', '"&amp;FragenTemplate!G62&amp;"', '"&amp;FragenTemplate!I62&amp;"', '"&amp;FragenTemplate!K62&amp;"', '"&amp;FragenTemplate!M62&amp;"', "&amp;IF(EXACT(FragenTemplate!H62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L62,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N62,"richtig"),"true","false")&amp;",true)"&amp;IF(A62="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C64),"",("('"&amp;FragenTemplate!C64&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D64),"","'"&amp;FragenTemplate!D64&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E64,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F64&amp;"', '"&amp;FragenTemplate!G64&amp;"', '"&amp;FragenTemplate!I64&amp;"', '"&amp;FragenTemplate!K64&amp;"', '"&amp;FragenTemplate!M64&amp;"', "&amp;IF(EXACT(FragenTemplate!H64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N64,"richtig"),"true","false")&amp;",true)"&amp;IF(A63="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C63),"",("('"&amp;FragenTemplate!C63&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D63),"","'"&amp;FragenTemplate!D63&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E63,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F63&amp;"', '"&amp;FragenTemplate!G63&amp;"', '"&amp;FragenTemplate!I63&amp;"', '"&amp;FragenTemplate!K63&amp;"', '"&amp;FragenTemplate!M63&amp;"', "&amp;IF(EXACT(FragenTemplate!H63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L63,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N63,"richtig"),"true","false")&amp;",true)"&amp;IF(A63="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C65),"",("('"&amp;FragenTemplate!C65&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D65),"","'"&amp;FragenTemplate!D65&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E65,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F65&amp;"', '"&amp;FragenTemplate!G65&amp;"', '"&amp;FragenTemplate!I65&amp;"', '"&amp;FragenTemplate!K65&amp;"', '"&amp;FragenTemplate!M65&amp;"', "&amp;IF(EXACT(FragenTemplate!H65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N65,"richtig"),"true","false")&amp;",true)"&amp;IF(A64="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C64),"",("('"&amp;FragenTemplate!C64&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D64),"","'"&amp;FragenTemplate!D64&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E64,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F64&amp;"', '"&amp;FragenTemplate!G64&amp;"', '"&amp;FragenTemplate!I64&amp;"', '"&amp;FragenTemplate!K64&amp;"', '"&amp;FragenTemplate!M64&amp;"', "&amp;IF(EXACT(FragenTemplate!H64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L64,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N64,"richtig"),"true","false")&amp;",true)"&amp;IF(A64="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C66),"",("('"&amp;FragenTemplate!C66&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D66),"","'"&amp;FragenTemplate!D66&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E66,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F66&amp;"', '"&amp;FragenTemplate!G66&amp;"', '"&amp;FragenTemplate!I66&amp;"', '"&amp;FragenTemplate!K66&amp;"', '"&amp;FragenTemplate!M66&amp;"', "&amp;IF(EXACT(FragenTemplate!H66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N66,"richtig"),"true","false")&amp;",true)"&amp;IF(A65="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C65),"",("('"&amp;FragenTemplate!C65&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D65),"","'"&amp;FragenTemplate!D65&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E65,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F65&amp;"', '"&amp;FragenTemplate!G65&amp;"', '"&amp;FragenTemplate!I65&amp;"', '"&amp;FragenTemplate!K65&amp;"', '"&amp;FragenTemplate!M65&amp;"', "&amp;IF(EXACT(FragenTemplate!H65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L65,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N65,"richtig"),"true","false")&amp;",true)"&amp;IF(A65="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C67),"",("('"&amp;FragenTemplate!C67&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D67),"","'"&amp;FragenTemplate!D67&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E67,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F67&amp;"', '"&amp;FragenTemplate!G67&amp;"', '"&amp;FragenTemplate!I67&amp;"', '"&amp;FragenTemplate!K67&amp;"', '"&amp;FragenTemplate!M67&amp;"', "&amp;IF(EXACT(FragenTemplate!H67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N67,"richtig"),"true","false")&amp;",true)"&amp;IF(A66="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C66),"",("('"&amp;FragenTemplate!C66&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D66),"","'"&amp;FragenTemplate!D66&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E66,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F66&amp;"', '"&amp;FragenTemplate!G66&amp;"', '"&amp;FragenTemplate!I66&amp;"', '"&amp;FragenTemplate!K66&amp;"', '"&amp;FragenTemplate!M66&amp;"', "&amp;IF(EXACT(FragenTemplate!H66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L66,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N66,"richtig"),"true","false")&amp;",true)"&amp;IF(A66="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C68),"",("('"&amp;FragenTemplate!C68&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D68),"","'"&amp;FragenTemplate!D68&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E68,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F68&amp;"', '"&amp;FragenTemplate!G68&amp;"', '"&amp;FragenTemplate!I68&amp;"', '"&amp;FragenTemplate!K68&amp;"', '"&amp;FragenTemplate!M68&amp;"', "&amp;IF(EXACT(FragenTemplate!H68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N68,"richtig"),"true","false")&amp;",true)"&amp;IF(A67="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C67),"",("('"&amp;FragenTemplate!C67&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D67),"","'"&amp;FragenTemplate!D67&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E67,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F67&amp;"', '"&amp;FragenTemplate!G67&amp;"', '"&amp;FragenTemplate!I67&amp;"', '"&amp;FragenTemplate!K67&amp;"', '"&amp;FragenTemplate!M67&amp;"', "&amp;IF(EXACT(FragenTemplate!H67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L67,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N67,"richtig"),"true","false")&amp;",true)"&amp;IF(A67="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C69),"",("('"&amp;FragenTemplate!C69&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D69),"","'"&amp;FragenTemplate!D69&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E69,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F69&amp;"', '"&amp;FragenTemplate!G69&amp;"', '"&amp;FragenTemplate!I69&amp;"', '"&amp;FragenTemplate!K69&amp;"', '"&amp;FragenTemplate!M69&amp;"', "&amp;IF(EXACT(FragenTemplate!H69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N69,"richtig"),"true","false")&amp;",true)"&amp;IF(A68="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C68),"",("('"&amp;FragenTemplate!C68&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D68),"","'"&amp;FragenTemplate!D68&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E68,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F68&amp;"', '"&amp;FragenTemplate!G68&amp;"', '"&amp;FragenTemplate!I68&amp;"', '"&amp;FragenTemplate!K68&amp;"', '"&amp;FragenTemplate!M68&amp;"', "&amp;IF(EXACT(FragenTemplate!H68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L68,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N68,"richtig"),"true","false")&amp;",true)"&amp;IF(A68="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C70),"",("('"&amp;FragenTemplate!C70&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D70),"","'"&amp;FragenTemplate!D70&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E70,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F70&amp;"', '"&amp;FragenTemplate!G70&amp;"', '"&amp;FragenTemplate!I70&amp;"', '"&amp;FragenTemplate!K70&amp;"', '"&amp;FragenTemplate!M70&amp;"', "&amp;IF(EXACT(FragenTemplate!H70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N70,"richtig"),"true","false")&amp;",true)"&amp;IF(A69="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C69),"",("('"&amp;FragenTemplate!C69&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D69),"","'"&amp;FragenTemplate!D69&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E69,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F69&amp;"', '"&amp;FragenTemplate!G69&amp;"', '"&amp;FragenTemplate!I69&amp;"', '"&amp;FragenTemplate!K69&amp;"', '"&amp;FragenTemplate!M69&amp;"', "&amp;IF(EXACT(FragenTemplate!H69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L69,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N69,"richtig"),"true","false")&amp;",true)"&amp;IF(A69="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C71),"",("('"&amp;FragenTemplate!C71&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D71),"","'"&amp;FragenTemplate!D71&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E71,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F71&amp;"', '"&amp;FragenTemplate!G71&amp;"', '"&amp;FragenTemplate!I71&amp;"', '"&amp;FragenTemplate!K71&amp;"', '"&amp;FragenTemplate!M71&amp;"', "&amp;IF(EXACT(FragenTemplate!H71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N71,"richtig"),"true","false")&amp;",true)"&amp;IF(A70="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C70),"",("('"&amp;FragenTemplate!C70&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D70),"","'"&amp;FragenTemplate!D70&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E70,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F70&amp;"', '"&amp;FragenTemplate!G70&amp;"', '"&amp;FragenTemplate!I70&amp;"', '"&amp;FragenTemplate!K70&amp;"', '"&amp;FragenTemplate!M70&amp;"', "&amp;IF(EXACT(FragenTemplate!H70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L70,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N70,"richtig"),"true","false")&amp;",true)"&amp;IF(A70="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C72),"",("('"&amp;FragenTemplate!C72&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D72),"","'"&amp;FragenTemplate!D72&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E72,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F72&amp;"', '"&amp;FragenTemplate!G72&amp;"', '"&amp;FragenTemplate!I72&amp;"', '"&amp;FragenTemplate!K72&amp;"', '"&amp;FragenTemplate!M72&amp;"', "&amp;IF(EXACT(FragenTemplate!H72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N72,"richtig"),"true","false")&amp;",true)"&amp;IF(A71="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C71),"",("('"&amp;FragenTemplate!C71&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D71),"","'"&amp;FragenTemplate!D71&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E71,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F71&amp;"', '"&amp;FragenTemplate!G71&amp;"', '"&amp;FragenTemplate!I71&amp;"', '"&amp;FragenTemplate!K71&amp;"', '"&amp;FragenTemplate!M71&amp;"', "&amp;IF(EXACT(FragenTemplate!H71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L71,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N71,"richtig"),"true","false")&amp;",true)"&amp;IF(A71="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C73),"",("('"&amp;FragenTemplate!C73&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D73),"","'"&amp;FragenTemplate!D73&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E73,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F73&amp;"', '"&amp;FragenTemplate!G73&amp;"', '"&amp;FragenTemplate!I73&amp;"', '"&amp;FragenTemplate!K73&amp;"', '"&amp;FragenTemplate!M73&amp;"', "&amp;IF(EXACT(FragenTemplate!H73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N73,"richtig"),"true","false")&amp;",true)"&amp;IF(A72="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C72),"",("('"&amp;FragenTemplate!C72&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D72),"","'"&amp;FragenTemplate!D72&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E72,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F72&amp;"', '"&amp;FragenTemplate!G72&amp;"', '"&amp;FragenTemplate!I72&amp;"', '"&amp;FragenTemplate!K72&amp;"', '"&amp;FragenTemplate!M72&amp;"', "&amp;IF(EXACT(FragenTemplate!H72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L72,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N72,"richtig"),"true","false")&amp;",true)"&amp;IF(A72="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C74),"",("('"&amp;FragenTemplate!C74&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D74),"","'"&amp;FragenTemplate!D74&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E74,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F74&amp;"', '"&amp;FragenTemplate!G74&amp;"', '"&amp;FragenTemplate!I74&amp;"', '"&amp;FragenTemplate!K74&amp;"', '"&amp;FragenTemplate!M74&amp;"', "&amp;IF(EXACT(FragenTemplate!H74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N74,"richtig"),"true","false")&amp;",true)"&amp;IF(A73="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C73),"",("('"&amp;FragenTemplate!C73&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D73),"","'"&amp;FragenTemplate!D73&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E73,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F73&amp;"', '"&amp;FragenTemplate!G73&amp;"', '"&amp;FragenTemplate!I73&amp;"', '"&amp;FragenTemplate!K73&amp;"', '"&amp;FragenTemplate!M73&amp;"', "&amp;IF(EXACT(FragenTemplate!H73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L73,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N73,"richtig"),"true","false")&amp;",true)"&amp;IF(A73="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C75),"",("('"&amp;FragenTemplate!C75&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D75),"","'"&amp;FragenTemplate!D75&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E75,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F75&amp;"', '"&amp;FragenTemplate!G75&amp;"', '"&amp;FragenTemplate!I75&amp;"', '"&amp;FragenTemplate!K75&amp;"', '"&amp;FragenTemplate!M75&amp;"', "&amp;IF(EXACT(FragenTemplate!H75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N75,"richtig"),"true","false")&amp;",true)"&amp;IF(A74="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C74),"",("('"&amp;FragenTemplate!C74&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D74),"","'"&amp;FragenTemplate!D74&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E74,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F74&amp;"', '"&amp;FragenTemplate!G74&amp;"', '"&amp;FragenTemplate!I74&amp;"', '"&amp;FragenTemplate!K74&amp;"', '"&amp;FragenTemplate!M74&amp;"', "&amp;IF(EXACT(FragenTemplate!H74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L74,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N74,"richtig"),"true","false")&amp;",true)"&amp;IF(A74="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C76),"",("('"&amp;FragenTemplate!C76&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D76),"","'"&amp;FragenTemplate!D76&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E76,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F76&amp;"', '"&amp;FragenTemplate!G76&amp;"', '"&amp;FragenTemplate!I76&amp;"', '"&amp;FragenTemplate!K76&amp;"', '"&amp;FragenTemplate!M76&amp;"', "&amp;IF(EXACT(FragenTemplate!H76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N76,"richtig"),"true","false")&amp;",true)"&amp;IF(A75="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C75),"",("('"&amp;FragenTemplate!C75&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D75),"","'"&amp;FragenTemplate!D75&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E75,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F75&amp;"', '"&amp;FragenTemplate!G75&amp;"', '"&amp;FragenTemplate!I75&amp;"', '"&amp;FragenTemplate!K75&amp;"', '"&amp;FragenTemplate!M75&amp;"', "&amp;IF(EXACT(FragenTemplate!H75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L75,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N75,"richtig"),"true","false")&amp;",true)"&amp;IF(A75="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C77),"",("('"&amp;FragenTemplate!C77&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D77),"","'"&amp;FragenTemplate!D77&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E77,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F77&amp;"', '"&amp;FragenTemplate!G77&amp;"', '"&amp;FragenTemplate!I77&amp;"', '"&amp;FragenTemplate!K77&amp;"', '"&amp;FragenTemplate!M77&amp;"', "&amp;IF(EXACT(FragenTemplate!H77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N77,"richtig"),"true","false")&amp;",true)"&amp;IF(A76="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C76),"",("('"&amp;FragenTemplate!C76&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D76),"","'"&amp;FragenTemplate!D76&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E76,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F76&amp;"', '"&amp;FragenTemplate!G76&amp;"', '"&amp;FragenTemplate!I76&amp;"', '"&amp;FragenTemplate!K76&amp;"', '"&amp;FragenTemplate!M76&amp;"', "&amp;IF(EXACT(FragenTemplate!H76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L76,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N76,"richtig"),"true","false")&amp;",true)"&amp;IF(A76="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C78),"",("('"&amp;FragenTemplate!C78&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D78),"","'"&amp;FragenTemplate!D78&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E78,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F78&amp;"', '"&amp;FragenTemplate!G78&amp;"', '"&amp;FragenTemplate!I78&amp;"', '"&amp;FragenTemplate!K78&amp;"', '"&amp;FragenTemplate!M78&amp;"', "&amp;IF(EXACT(FragenTemplate!H78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N78,"richtig"),"true","false")&amp;",true)"&amp;IF(A77="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C77),"",("('"&amp;FragenTemplate!C77&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D77),"","'"&amp;FragenTemplate!D77&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E77,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F77&amp;"', '"&amp;FragenTemplate!G77&amp;"', '"&amp;FragenTemplate!I77&amp;"', '"&amp;FragenTemplate!K77&amp;"', '"&amp;FragenTemplate!M77&amp;"', "&amp;IF(EXACT(FragenTemplate!H77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L77,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N77,"richtig"),"true","false")&amp;",true)"&amp;IF(A77="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C79),"",("('"&amp;FragenTemplate!C79&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D79),"","'"&amp;FragenTemplate!D79&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E79,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F79&amp;"', '"&amp;FragenTemplate!G79&amp;"', '"&amp;FragenTemplate!I79&amp;"', '"&amp;FragenTemplate!K79&amp;"', '"&amp;FragenTemplate!M79&amp;"', "&amp;IF(EXACT(FragenTemplate!H79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N79,"richtig"),"true","false")&amp;",true)"&amp;IF(A78="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C78),"",("('"&amp;FragenTemplate!C78&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D78),"","'"&amp;FragenTemplate!D78&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E78,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F78&amp;"', '"&amp;FragenTemplate!G78&amp;"', '"&amp;FragenTemplate!I78&amp;"', '"&amp;FragenTemplate!K78&amp;"', '"&amp;FragenTemplate!M78&amp;"', "&amp;IF(EXACT(FragenTemplate!H78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L78,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N78,"richtig"),"true","false")&amp;",true)"&amp;IF(A78="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C80),"",("('"&amp;FragenTemplate!C80&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D80),"","'"&amp;FragenTemplate!D80&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E80,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F80&amp;"', '"&amp;FragenTemplate!G80&amp;"', '"&amp;FragenTemplate!I80&amp;"', '"&amp;FragenTemplate!K80&amp;"', '"&amp;FragenTemplate!M80&amp;"', "&amp;IF(EXACT(FragenTemplate!H80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N80,"richtig"),"true","false")&amp;",true)"&amp;IF(A79="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C79),"",("('"&amp;FragenTemplate!C79&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D79),"","'"&amp;FragenTemplate!D79&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E79,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F79&amp;"', '"&amp;FragenTemplate!G79&amp;"', '"&amp;FragenTemplate!I79&amp;"', '"&amp;FragenTemplate!K79&amp;"', '"&amp;FragenTemplate!M79&amp;"', "&amp;IF(EXACT(FragenTemplate!H79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L79,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N79,"richtig"),"true","false")&amp;",true)"&amp;IF(A79="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C81),"",("('"&amp;FragenTemplate!C81&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D81),"","'"&amp;FragenTemplate!D81&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E81,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F81&amp;"', '"&amp;FragenTemplate!G81&amp;"', '"&amp;FragenTemplate!I81&amp;"', '"&amp;FragenTemplate!K81&amp;"', '"&amp;FragenTemplate!M81&amp;"', "&amp;IF(EXACT(FragenTemplate!H81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N81,"richtig"),"true","false")&amp;",true)"&amp;IF(A80="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C80),"",("('"&amp;FragenTemplate!C80&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D80),"","'"&amp;FragenTemplate!D80&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E80,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F80&amp;"', '"&amp;FragenTemplate!G80&amp;"', '"&amp;FragenTemplate!I80&amp;"', '"&amp;FragenTemplate!K80&amp;"', '"&amp;FragenTemplate!M80&amp;"', "&amp;IF(EXACT(FragenTemplate!H80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L80,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N80,"richtig"),"true","false")&amp;",true)"&amp;IF(A80="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C82),"",("('"&amp;FragenTemplate!C82&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D82),"","'"&amp;FragenTemplate!D82&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E82,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F82&amp;"', '"&amp;FragenTemplate!G82&amp;"', '"&amp;FragenTemplate!I82&amp;"', '"&amp;FragenTemplate!K82&amp;"', '"&amp;FragenTemplate!M82&amp;"', "&amp;IF(EXACT(FragenTemplate!H82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N82,"richtig"),"true","false")&amp;",true)"&amp;IF(A81="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C81),"",("('"&amp;FragenTemplate!C81&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D81),"","'"&amp;FragenTemplate!D81&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E81,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F81&amp;"', '"&amp;FragenTemplate!G81&amp;"', '"&amp;FragenTemplate!I81&amp;"', '"&amp;FragenTemplate!K81&amp;"', '"&amp;FragenTemplate!M81&amp;"', "&amp;IF(EXACT(FragenTemplate!H81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L81,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N81,"richtig"),"true","false")&amp;",true)"&amp;IF(A81="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C83),"",("('"&amp;FragenTemplate!C83&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D83),"","'"&amp;FragenTemplate!D83&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E83,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F83&amp;"', '"&amp;FragenTemplate!G83&amp;"', '"&amp;FragenTemplate!I83&amp;"', '"&amp;FragenTemplate!K83&amp;"', '"&amp;FragenTemplate!M83&amp;"', "&amp;IF(EXACT(FragenTemplate!H83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N83,"richtig"),"true","false")&amp;",true)"&amp;IF(A82="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C82),"",("('"&amp;FragenTemplate!C82&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D82),"","'"&amp;FragenTemplate!D82&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E82,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F82&amp;"', '"&amp;FragenTemplate!G82&amp;"', '"&amp;FragenTemplate!I82&amp;"', '"&amp;FragenTemplate!K82&amp;"', '"&amp;FragenTemplate!M82&amp;"', "&amp;IF(EXACT(FragenTemplate!H82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L82,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N82,"richtig"),"true","false")&amp;",true)"&amp;IF(A82="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C84),"",("('"&amp;FragenTemplate!C84&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D84),"","'"&amp;FragenTemplate!D84&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E84,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F84&amp;"', '"&amp;FragenTemplate!G84&amp;"', '"&amp;FragenTemplate!I84&amp;"', '"&amp;FragenTemplate!K84&amp;"', '"&amp;FragenTemplate!M84&amp;"', "&amp;IF(EXACT(FragenTemplate!H84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N84,"richtig"),"true","false")&amp;",true)"&amp;IF(A83="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C83),"",("('"&amp;FragenTemplate!C83&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D83),"","'"&amp;FragenTemplate!D83&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E83,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F83&amp;"', '"&amp;FragenTemplate!G83&amp;"', '"&amp;FragenTemplate!I83&amp;"', '"&amp;FragenTemplate!K83&amp;"', '"&amp;FragenTemplate!M83&amp;"', "&amp;IF(EXACT(FragenTemplate!H83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L83,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N83,"richtig"),"true","false")&amp;",true)"&amp;IF(A83="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C85),"",("('"&amp;FragenTemplate!C85&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D85),"","'"&amp;FragenTemplate!D85&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E85,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F85&amp;"', '"&amp;FragenTemplate!G85&amp;"', '"&amp;FragenTemplate!I85&amp;"', '"&amp;FragenTemplate!K85&amp;"', '"&amp;FragenTemplate!M85&amp;"', "&amp;IF(EXACT(FragenTemplate!H85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N85,"richtig"),"true","false")&amp;",true)"&amp;IF(A84="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C84),"",("('"&amp;FragenTemplate!C84&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D84),"","'"&amp;FragenTemplate!D84&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E84,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F84&amp;"', '"&amp;FragenTemplate!G84&amp;"', '"&amp;FragenTemplate!I84&amp;"', '"&amp;FragenTemplate!K84&amp;"', '"&amp;FragenTemplate!M84&amp;"', "&amp;IF(EXACT(FragenTemplate!H84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L84,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N84,"richtig"),"true","false")&amp;",true)"&amp;IF(A84="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C86),"",("('"&amp;FragenTemplate!C86&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D86),"","'"&amp;FragenTemplate!D86&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E86,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F86&amp;"', '"&amp;FragenTemplate!G86&amp;"', '"&amp;FragenTemplate!I86&amp;"', '"&amp;FragenTemplate!K86&amp;"', '"&amp;FragenTemplate!M86&amp;"', "&amp;IF(EXACT(FragenTemplate!H86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N86,"richtig"),"true","false")&amp;",true)"&amp;IF(A85="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C85),"",("('"&amp;FragenTemplate!C85&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D85),"","'"&amp;FragenTemplate!D85&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E85,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F85&amp;"', '"&amp;FragenTemplate!G85&amp;"', '"&amp;FragenTemplate!I85&amp;"', '"&amp;FragenTemplate!K85&amp;"', '"&amp;FragenTemplate!M85&amp;"', "&amp;IF(EXACT(FragenTemplate!H85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L85,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N85,"richtig"),"true","false")&amp;",true)"&amp;IF(A85="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C87),"",("('"&amp;FragenTemplate!C87&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D87),"","'"&amp;FragenTemplate!D87&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E87,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F87&amp;"', '"&amp;FragenTemplate!G87&amp;"', '"&amp;FragenTemplate!I87&amp;"', '"&amp;FragenTemplate!K87&amp;"', '"&amp;FragenTemplate!M87&amp;"', "&amp;IF(EXACT(FragenTemplate!H87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N87,"richtig"),"true","false")&amp;",true)"&amp;IF(A86="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C86),"",("('"&amp;FragenTemplate!C86&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D86),"","'"&amp;FragenTemplate!D86&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E86,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F86&amp;"', '"&amp;FragenTemplate!G86&amp;"', '"&amp;FragenTemplate!I86&amp;"', '"&amp;FragenTemplate!K86&amp;"', '"&amp;FragenTemplate!M86&amp;"', "&amp;IF(EXACT(FragenTemplate!H86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L86,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N86,"richtig"),"true","false")&amp;",true)"&amp;IF(A86="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C88),"",("('"&amp;FragenTemplate!C88&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D88),"","'"&amp;FragenTemplate!D88&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E88,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F88&amp;"', '"&amp;FragenTemplate!G88&amp;"', '"&amp;FragenTemplate!I88&amp;"', '"&amp;FragenTemplate!K88&amp;"', '"&amp;FragenTemplate!M88&amp;"', "&amp;IF(EXACT(FragenTemplate!H88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N88,"richtig"),"true","false")&amp;",true)"&amp;IF(A87="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C87),"",("('"&amp;FragenTemplate!C87&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D87),"","'"&amp;FragenTemplate!D87&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E87,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F87&amp;"', '"&amp;FragenTemplate!G87&amp;"', '"&amp;FragenTemplate!I87&amp;"', '"&amp;FragenTemplate!K87&amp;"', '"&amp;FragenTemplate!M87&amp;"', "&amp;IF(EXACT(FragenTemplate!H87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L87,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N87,"richtig"),"true","false")&amp;",true)"&amp;IF(A87="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C89),"",("('"&amp;FragenTemplate!C89&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D89),"","'"&amp;FragenTemplate!D89&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E89,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F89&amp;"', '"&amp;FragenTemplate!G89&amp;"', '"&amp;FragenTemplate!I89&amp;"', '"&amp;FragenTemplate!K89&amp;"', '"&amp;FragenTemplate!M89&amp;"', "&amp;IF(EXACT(FragenTemplate!H89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N89,"richtig"),"true","false")&amp;",true)"&amp;IF(A88="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C88),"",("('"&amp;FragenTemplate!C88&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D88),"","'"&amp;FragenTemplate!D88&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E88,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F88&amp;"', '"&amp;FragenTemplate!G88&amp;"', '"&amp;FragenTemplate!I88&amp;"', '"&amp;FragenTemplate!K88&amp;"', '"&amp;FragenTemplate!M88&amp;"', "&amp;IF(EXACT(FragenTemplate!H88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L88,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N88,"richtig"),"true","false")&amp;",true)"&amp;IF(A88="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C90),"",("('"&amp;FragenTemplate!C90&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D90),"","'"&amp;FragenTemplate!D90&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E90,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F90&amp;"', '"&amp;FragenTemplate!G90&amp;"', '"&amp;FragenTemplate!I90&amp;"', '"&amp;FragenTemplate!K90&amp;"', '"&amp;FragenTemplate!M90&amp;"', "&amp;IF(EXACT(FragenTemplate!H90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N90,"richtig"),"true","false")&amp;",true)"&amp;IF(A89="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C89),"",("('"&amp;FragenTemplate!C89&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D89),"","'"&amp;FragenTemplate!D89&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E89,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F89&amp;"', '"&amp;FragenTemplate!G89&amp;"', '"&amp;FragenTemplate!I89&amp;"', '"&amp;FragenTemplate!K89&amp;"', '"&amp;FragenTemplate!M89&amp;"', "&amp;IF(EXACT(FragenTemplate!H89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L89,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N89,"richtig"),"true","false")&amp;",true)"&amp;IF(A89="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C91),"",("('"&amp;FragenTemplate!C91&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D91),"","'"&amp;FragenTemplate!D91&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E91,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F91&amp;"', '"&amp;FragenTemplate!G91&amp;"', '"&amp;FragenTemplate!I91&amp;"', '"&amp;FragenTemplate!K91&amp;"', '"&amp;FragenTemplate!M91&amp;"', "&amp;IF(EXACT(FragenTemplate!H91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N91,"richtig"),"true","false")&amp;",true)"&amp;IF(A90="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C90),"",("('"&amp;FragenTemplate!C90&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D90),"","'"&amp;FragenTemplate!D90&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E90,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F90&amp;"', '"&amp;FragenTemplate!G90&amp;"', '"&amp;FragenTemplate!I90&amp;"', '"&amp;FragenTemplate!K90&amp;"', '"&amp;FragenTemplate!M90&amp;"', "&amp;IF(EXACT(FragenTemplate!H90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L90,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N90,"richtig"),"true","false")&amp;",true)"&amp;IF(A90="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C92),"",("('"&amp;FragenTemplate!C92&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D92),"","'"&amp;FragenTemplate!D92&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E92,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F92&amp;"', '"&amp;FragenTemplate!G92&amp;"', '"&amp;FragenTemplate!I92&amp;"', '"&amp;FragenTemplate!K92&amp;"', '"&amp;FragenTemplate!M92&amp;"', "&amp;IF(EXACT(FragenTemplate!H92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N92,"richtig"),"true","false")&amp;",true)"&amp;IF(A91="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C91),"",("('"&amp;FragenTemplate!C91&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D91),"","'"&amp;FragenTemplate!D91&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E91,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F91&amp;"', '"&amp;FragenTemplate!G91&amp;"', '"&amp;FragenTemplate!I91&amp;"', '"&amp;FragenTemplate!K91&amp;"', '"&amp;FragenTemplate!M91&amp;"', "&amp;IF(EXACT(FragenTemplate!H91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L91,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N91,"richtig"),"true","false")&amp;",true)"&amp;IF(A91="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C93),"",("('"&amp;FragenTemplate!C93&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D93),"","'"&amp;FragenTemplate!D93&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E93,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F93&amp;"', '"&amp;FragenTemplate!G93&amp;"', '"&amp;FragenTemplate!I93&amp;"', '"&amp;FragenTemplate!K93&amp;"', '"&amp;FragenTemplate!M93&amp;"', "&amp;IF(EXACT(FragenTemplate!H93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N93,"richtig"),"true","false")&amp;",true)"&amp;IF(A92="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C92),"",("('"&amp;FragenTemplate!C92&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D92),"","'"&amp;FragenTemplate!D92&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E92,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F92&amp;"', '"&amp;FragenTemplate!G92&amp;"', '"&amp;FragenTemplate!I92&amp;"', '"&amp;FragenTemplate!K92&amp;"', '"&amp;FragenTemplate!M92&amp;"', "&amp;IF(EXACT(FragenTemplate!H92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L92,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N92,"richtig"),"true","false")&amp;",true)"&amp;IF(A92="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C94),"",("('"&amp;FragenTemplate!C94&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D94),"","'"&amp;FragenTemplate!D94&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E94,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F94&amp;"', '"&amp;FragenTemplate!G94&amp;"', '"&amp;FragenTemplate!I94&amp;"', '"&amp;FragenTemplate!K94&amp;"', '"&amp;FragenTemplate!M94&amp;"', "&amp;IF(EXACT(FragenTemplate!H94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N94,"richtig"),"true","false")&amp;",true)"&amp;IF(A93="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C93),"",("('"&amp;FragenTemplate!C93&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D93),"","'"&amp;FragenTemplate!D93&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E93,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F93&amp;"', '"&amp;FragenTemplate!G93&amp;"', '"&amp;FragenTemplate!I93&amp;"', '"&amp;FragenTemplate!K93&amp;"', '"&amp;FragenTemplate!M93&amp;"', "&amp;IF(EXACT(FragenTemplate!H93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L93,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N93,"richtig"),"true","false")&amp;",true)"&amp;IF(A93="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C95),"",("('"&amp;FragenTemplate!C95&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D95),"","'"&amp;FragenTemplate!D95&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E95,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F95&amp;"', '"&amp;FragenTemplate!G95&amp;"', '"&amp;FragenTemplate!I95&amp;"', '"&amp;FragenTemplate!K95&amp;"', '"&amp;FragenTemplate!M95&amp;"', "&amp;IF(EXACT(FragenTemplate!H95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N95,"richtig"),"true","false")&amp;",true)"&amp;IF(A94="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C94),"",("('"&amp;FragenTemplate!C94&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D94),"","'"&amp;FragenTemplate!D94&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E94,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F94&amp;"', '"&amp;FragenTemplate!G94&amp;"', '"&amp;FragenTemplate!I94&amp;"', '"&amp;FragenTemplate!K94&amp;"', '"&amp;FragenTemplate!M94&amp;"', "&amp;IF(EXACT(FragenTemplate!H94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L94,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N94,"richtig"),"true","false")&amp;",true)"&amp;IF(A94="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C96),"",("('"&amp;FragenTemplate!C96&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D96),"","'"&amp;FragenTemplate!D96&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E96,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F96&amp;"', '"&amp;FragenTemplate!G96&amp;"', '"&amp;FragenTemplate!I96&amp;"', '"&amp;FragenTemplate!K96&amp;"', '"&amp;FragenTemplate!M96&amp;"', "&amp;IF(EXACT(FragenTemplate!H96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N96,"richtig"),"true","false")&amp;",true)"&amp;IF(A95="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C95),"",("('"&amp;FragenTemplate!C95&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D95),"","'"&amp;FragenTemplate!D95&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E95,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F95&amp;"', '"&amp;FragenTemplate!G95&amp;"', '"&amp;FragenTemplate!I95&amp;"', '"&amp;FragenTemplate!K95&amp;"', '"&amp;FragenTemplate!M95&amp;"', "&amp;IF(EXACT(FragenTemplate!H95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L95,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N95,"richtig"),"true","false")&amp;",true)"&amp;IF(A95="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C97),"",("('"&amp;FragenTemplate!C97&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D97),"","'"&amp;FragenTemplate!D97&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E97,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F97&amp;"', '"&amp;FragenTemplate!G97&amp;"', '"&amp;FragenTemplate!I97&amp;"', '"&amp;FragenTemplate!K97&amp;"', '"&amp;FragenTemplate!M97&amp;"', "&amp;IF(EXACT(FragenTemplate!H97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N97,"richtig"),"true","false")&amp;",true)"&amp;IF(A96="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C96),"",("('"&amp;FragenTemplate!C96&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D96),"","'"&amp;FragenTemplate!D96&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E96,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F96&amp;"', '"&amp;FragenTemplate!G96&amp;"', '"&amp;FragenTemplate!I96&amp;"', '"&amp;FragenTemplate!K96&amp;"', '"&amp;FragenTemplate!M96&amp;"', "&amp;IF(EXACT(FragenTemplate!H96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L96,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N96,"richtig"),"true","false")&amp;",true)"&amp;IF(A96="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C98),"",("('"&amp;FragenTemplate!C98&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D98),"","'"&amp;FragenTemplate!D98&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E98,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F98&amp;"', '"&amp;FragenTemplate!G98&amp;"', '"&amp;FragenTemplate!I98&amp;"', '"&amp;FragenTemplate!K98&amp;"', '"&amp;FragenTemplate!M98&amp;"', "&amp;IF(EXACT(FragenTemplate!H98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N98,"richtig"),"true","false")&amp;",true)"&amp;IF(A97="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C97),"",("('"&amp;FragenTemplate!C97&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D97),"","'"&amp;FragenTemplate!D97&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E97,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F97&amp;"', '"&amp;FragenTemplate!G97&amp;"', '"&amp;FragenTemplate!I97&amp;"', '"&amp;FragenTemplate!K97&amp;"', '"&amp;FragenTemplate!M97&amp;"', "&amp;IF(EXACT(FragenTemplate!H97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L97,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N97,"richtig"),"true","false")&amp;",true)"&amp;IF(A97="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C99),"",("('"&amp;FragenTemplate!C99&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D99),"","'"&amp;FragenTemplate!D99&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E99,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F99&amp;"', '"&amp;FragenTemplate!G99&amp;"', '"&amp;FragenTemplate!I99&amp;"', '"&amp;FragenTemplate!K99&amp;"', '"&amp;FragenTemplate!M99&amp;"', "&amp;IF(EXACT(FragenTemplate!H99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N99,"richtig"),"true","false")&amp;",true)"&amp;IF(A98="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C98),"",("('"&amp;FragenTemplate!C98&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D98),"","'"&amp;FragenTemplate!D98&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E98,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F98&amp;"', '"&amp;FragenTemplate!G98&amp;"', '"&amp;FragenTemplate!I98&amp;"', '"&amp;FragenTemplate!K98&amp;"', '"&amp;FragenTemplate!M98&amp;"', "&amp;IF(EXACT(FragenTemplate!H98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L98,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N98,"richtig"),"true","false")&amp;",true)"&amp;IF(A98="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C100),"",("('"&amp;FragenTemplate!C100&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D100),"","'"&amp;FragenTemplate!D100&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E100,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F100&amp;"', '"&amp;FragenTemplate!G100&amp;"', '"&amp;FragenTemplate!I100&amp;"', '"&amp;FragenTemplate!K100&amp;"', '"&amp;FragenTemplate!M100&amp;"', "&amp;IF(EXACT(FragenTemplate!H100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N100,"richtig"),"true","false")&amp;",true)"&amp;IF(A99="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C99),"",("('"&amp;FragenTemplate!C99&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D99),"","'"&amp;FragenTemplate!D99&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E99,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F99&amp;"', '"&amp;FragenTemplate!G99&amp;"', '"&amp;FragenTemplate!I99&amp;"', '"&amp;FragenTemplate!K99&amp;"', '"&amp;FragenTemplate!M99&amp;"', "&amp;IF(EXACT(FragenTemplate!H99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L99,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N99,"richtig"),"true","false")&amp;",true)"&amp;IF(A99="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C101),"",("('"&amp;FragenTemplate!C101&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D101),"","'"&amp;FragenTemplate!D101&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E101,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F101&amp;"', '"&amp;FragenTemplate!G101&amp;"', '"&amp;FragenTemplate!I101&amp;"', '"&amp;FragenTemplate!K101&amp;"', '"&amp;FragenTemplate!M101&amp;"', "&amp;IF(EXACT(FragenTemplate!H101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N101,"richtig"),"true","false")&amp;",true)"&amp;IF(A100="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C100),"",("('"&amp;FragenTemplate!C100&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D100),"","'"&amp;FragenTemplate!D100&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E100,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F100&amp;"', '"&amp;FragenTemplate!G100&amp;"', '"&amp;FragenTemplate!I100&amp;"', '"&amp;FragenTemplate!K100&amp;"', '"&amp;FragenTemplate!M100&amp;"', "&amp;IF(EXACT(FragenTemplate!H100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L100,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N100,"richtig"),"true","false")&amp;",true)"&amp;IF(A100="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C102),"",("('"&amp;FragenTemplate!C102&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D102),"","'"&amp;FragenTemplate!D102&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E102,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F102&amp;"', '"&amp;FragenTemplate!G102&amp;"', '"&amp;FragenTemplate!I102&amp;"', '"&amp;FragenTemplate!K102&amp;"', '"&amp;FragenTemplate!M102&amp;"', "&amp;IF(EXACT(FragenTemplate!H102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N102,"richtig"),"true","false")&amp;",true)"&amp;IF(A101="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C101),"",("('"&amp;FragenTemplate!C101&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D101),"","'"&amp;FragenTemplate!D101&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E101,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F101&amp;"', '"&amp;FragenTemplate!G101&amp;"', '"&amp;FragenTemplate!I101&amp;"', '"&amp;FragenTemplate!K101&amp;"', '"&amp;FragenTemplate!M101&amp;"', "&amp;IF(EXACT(FragenTemplate!H101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L101,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N101,"richtig"),"true","false")&amp;",true)"&amp;IF(A101="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C103),"",("('"&amp;FragenTemplate!C103&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D103),"","'"&amp;FragenTemplate!D103&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E103,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F103&amp;"', '"&amp;FragenTemplate!G103&amp;"', '"&amp;FragenTemplate!I103&amp;"', '"&amp;FragenTemplate!K103&amp;"', '"&amp;FragenTemplate!M103&amp;"', "&amp;IF(EXACT(FragenTemplate!H103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N103,"richtig"),"true","false")&amp;",true)"&amp;IF(A102="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C102),"",("('"&amp;FragenTemplate!C102&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D102),"","'"&amp;FragenTemplate!D102&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E102,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F102&amp;"', '"&amp;FragenTemplate!G102&amp;"', '"&amp;FragenTemplate!I102&amp;"', '"&amp;FragenTemplate!K102&amp;"', '"&amp;FragenTemplate!M102&amp;"', "&amp;IF(EXACT(FragenTemplate!H102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L102,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N102,"richtig"),"true","false")&amp;",true)"&amp;IF(A102="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C104),"",("('"&amp;FragenTemplate!C104&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D104),"","'"&amp;FragenTemplate!D104&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E104,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F104&amp;"', '"&amp;FragenTemplate!G104&amp;"', '"&amp;FragenTemplate!I104&amp;"', '"&amp;FragenTemplate!K104&amp;"', '"&amp;FragenTemplate!M104&amp;"', "&amp;IF(EXACT(FragenTemplate!H104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N104,"richtig"),"true","false")&amp;",true)"&amp;IF(A103="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C103),"",("('"&amp;FragenTemplate!C103&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D103),"","'"&amp;FragenTemplate!D103&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E103,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F103&amp;"', '"&amp;FragenTemplate!G103&amp;"', '"&amp;FragenTemplate!I103&amp;"', '"&amp;FragenTemplate!K103&amp;"', '"&amp;FragenTemplate!M103&amp;"', "&amp;IF(EXACT(FragenTemplate!H103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L103,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N103,"richtig"),"true","false")&amp;",true)"&amp;IF(A103="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C105),"",("('"&amp;FragenTemplate!C105&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D105),"","'"&amp;FragenTemplate!D105&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E105,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F105&amp;"', '"&amp;FragenTemplate!G105&amp;"', '"&amp;FragenTemplate!I105&amp;"', '"&amp;FragenTemplate!K105&amp;"', '"&amp;FragenTemplate!M105&amp;"', "&amp;IF(EXACT(FragenTemplate!H105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N105,"richtig"),"true","false")&amp;",true)"&amp;IF(A104="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C104),"",("('"&amp;FragenTemplate!C104&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D104),"","'"&amp;FragenTemplate!D104&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E104,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F104&amp;"', '"&amp;FragenTemplate!G104&amp;"', '"&amp;FragenTemplate!I104&amp;"', '"&amp;FragenTemplate!K104&amp;"', '"&amp;FragenTemplate!M104&amp;"', "&amp;IF(EXACT(FragenTemplate!H104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L104,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N104,"richtig"),"true","false")&amp;",true)"&amp;IF(A104="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C106),"",("('"&amp;FragenTemplate!C106&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D106),"","'"&amp;FragenTemplate!D106&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E106,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F106&amp;"', '"&amp;FragenTemplate!G106&amp;"', '"&amp;FragenTemplate!I106&amp;"', '"&amp;FragenTemplate!K106&amp;"', '"&amp;FragenTemplate!M106&amp;"', "&amp;IF(EXACT(FragenTemplate!H106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N106,"richtig"),"true","false")&amp;",true)"&amp;IF(A105="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C105),"",("('"&amp;FragenTemplate!C105&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D105),"","'"&amp;FragenTemplate!D105&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E105,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F105&amp;"', '"&amp;FragenTemplate!G105&amp;"', '"&amp;FragenTemplate!I105&amp;"', '"&amp;FragenTemplate!K105&amp;"', '"&amp;FragenTemplate!M105&amp;"', "&amp;IF(EXACT(FragenTemplate!H105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L105,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N105,"richtig"),"true","false")&amp;",true)"&amp;IF(A105="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C107),"",("('"&amp;FragenTemplate!C107&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D107),"","'"&amp;FragenTemplate!D107&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E107,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F107&amp;"', '"&amp;FragenTemplate!G107&amp;"', '"&amp;FragenTemplate!I107&amp;"', '"&amp;FragenTemplate!K107&amp;"', '"&amp;FragenTemplate!M107&amp;"', "&amp;IF(EXACT(FragenTemplate!H107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N107,"richtig"),"true","false")&amp;",true)"&amp;IF(A106="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C106),"",("('"&amp;FragenTemplate!C106&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D106),"","'"&amp;FragenTemplate!D106&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E106,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F106&amp;"', '"&amp;FragenTemplate!G106&amp;"', '"&amp;FragenTemplate!I106&amp;"', '"&amp;FragenTemplate!K106&amp;"', '"&amp;FragenTemplate!M106&amp;"', "&amp;IF(EXACT(FragenTemplate!H106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L106,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N106,"richtig"),"true","false")&amp;",true)"&amp;IF(A106="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C108),"",("('"&amp;FragenTemplate!C108&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D108),"","'"&amp;FragenTemplate!D108&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E108,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F108&amp;"', '"&amp;FragenTemplate!G108&amp;"', '"&amp;FragenTemplate!I108&amp;"', '"&amp;FragenTemplate!K108&amp;"', '"&amp;FragenTemplate!M108&amp;"', "&amp;IF(EXACT(FragenTemplate!H108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N108,"richtig"),"true","false")&amp;",true)"&amp;IF(A107="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C107),"",("('"&amp;FragenTemplate!C107&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D107),"","'"&amp;FragenTemplate!D107&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E107,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F107&amp;"', '"&amp;FragenTemplate!G107&amp;"', '"&amp;FragenTemplate!I107&amp;"', '"&amp;FragenTemplate!K107&amp;"', '"&amp;FragenTemplate!M107&amp;"', "&amp;IF(EXACT(FragenTemplate!H107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L107,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N107,"richtig"),"true","false")&amp;",true)"&amp;IF(A107="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C109),"",("('"&amp;FragenTemplate!C109&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D109),"","'"&amp;FragenTemplate!D109&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E109,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F109&amp;"', '"&amp;FragenTemplate!G109&amp;"', '"&amp;FragenTemplate!I109&amp;"', '"&amp;FragenTemplate!K109&amp;"', '"&amp;FragenTemplate!M109&amp;"', "&amp;IF(EXACT(FragenTemplate!H109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N109,"richtig"),"true","false")&amp;",true)"&amp;IF(A108="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C108),"",("('"&amp;FragenTemplate!C108&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D108),"","'"&amp;FragenTemplate!D108&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E108,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F108&amp;"', '"&amp;FragenTemplate!G108&amp;"', '"&amp;FragenTemplate!I108&amp;"', '"&amp;FragenTemplate!K108&amp;"', '"&amp;FragenTemplate!M108&amp;"', "&amp;IF(EXACT(FragenTemplate!H108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L108,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N108,"richtig"),"true","false")&amp;",true)"&amp;IF(A108="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C110),"",("('"&amp;FragenTemplate!C110&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D110),"","'"&amp;FragenTemplate!D110&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E110,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F110&amp;"', '"&amp;FragenTemplate!G110&amp;"', '"&amp;FragenTemplate!I110&amp;"', '"&amp;FragenTemplate!K110&amp;"', '"&amp;FragenTemplate!M110&amp;"', "&amp;IF(EXACT(FragenTemplate!H110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N110,"richtig"),"true","false")&amp;",true)"&amp;IF(A109="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C109),"",("('"&amp;FragenTemplate!C109&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D109),"","'"&amp;FragenTemplate!D109&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E109,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F109&amp;"', '"&amp;FragenTemplate!G109&amp;"', '"&amp;FragenTemplate!I109&amp;"', '"&amp;FragenTemplate!K109&amp;"', '"&amp;FragenTemplate!M109&amp;"', "&amp;IF(EXACT(FragenTemplate!H109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L109,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N109,"richtig"),"true","false")&amp;",true)"&amp;IF(A109="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C111),"",("('"&amp;FragenTemplate!C111&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D111),"","'"&amp;FragenTemplate!D111&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E111,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F111&amp;"', '"&amp;FragenTemplate!G111&amp;"', '"&amp;FragenTemplate!I111&amp;"', '"&amp;FragenTemplate!K111&amp;"', '"&amp;FragenTemplate!M111&amp;"', "&amp;IF(EXACT(FragenTemplate!H111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N111,"richtig"),"true","false")&amp;",true)"&amp;IF(A110="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C110),"",("('"&amp;FragenTemplate!C110&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D110),"","'"&amp;FragenTemplate!D110&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E110,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F110&amp;"', '"&amp;FragenTemplate!G110&amp;"', '"&amp;FragenTemplate!I110&amp;"', '"&amp;FragenTemplate!K110&amp;"', '"&amp;FragenTemplate!M110&amp;"', "&amp;IF(EXACT(FragenTemplate!H110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L110,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N110,"richtig"),"true","false")&amp;",true)"&amp;IF(A110="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C112),"",("('"&amp;FragenTemplate!C112&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D112),"","'"&amp;FragenTemplate!D112&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E112,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F112&amp;"', '"&amp;FragenTemplate!G112&amp;"', '"&amp;FragenTemplate!I112&amp;"', '"&amp;FragenTemplate!K112&amp;"', '"&amp;FragenTemplate!M112&amp;"', "&amp;IF(EXACT(FragenTemplate!H112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N112,"richtig"),"true","false")&amp;",true)"&amp;IF(A111="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C111),"",("('"&amp;FragenTemplate!C111&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D111),"","'"&amp;FragenTemplate!D111&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E111,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F111&amp;"', '"&amp;FragenTemplate!G111&amp;"', '"&amp;FragenTemplate!I111&amp;"', '"&amp;FragenTemplate!K111&amp;"', '"&amp;FragenTemplate!M111&amp;"', "&amp;IF(EXACT(FragenTemplate!H111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L111,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N111,"richtig"),"true","false")&amp;",true)"&amp;IF(A111="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C113),"",("('"&amp;FragenTemplate!C113&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D113),"","'"&amp;FragenTemplate!D113&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E113,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F113&amp;"', '"&amp;FragenTemplate!G113&amp;"', '"&amp;FragenTemplate!I113&amp;"', '"&amp;FragenTemplate!K113&amp;"', '"&amp;FragenTemplate!M113&amp;"', "&amp;IF(EXACT(FragenTemplate!H113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N113,"richtig"),"true","false")&amp;",true)"&amp;IF(A112="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C112),"",("('"&amp;FragenTemplate!C112&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D112),"","'"&amp;FragenTemplate!D112&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E112,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F112&amp;"', '"&amp;FragenTemplate!G112&amp;"', '"&amp;FragenTemplate!I112&amp;"', '"&amp;FragenTemplate!K112&amp;"', '"&amp;FragenTemplate!M112&amp;"', "&amp;IF(EXACT(FragenTemplate!H112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L112,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N112,"richtig"),"true","false")&amp;",true)"&amp;IF(A112="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C114),"",("('"&amp;FragenTemplate!C114&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D114),"","'"&amp;FragenTemplate!D114&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E114,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F114&amp;"', '"&amp;FragenTemplate!G114&amp;"', '"&amp;FragenTemplate!I114&amp;"', '"&amp;FragenTemplate!K114&amp;"', '"&amp;FragenTemplate!M114&amp;"', "&amp;IF(EXACT(FragenTemplate!H114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N114,"richtig"),"true","false")&amp;",true)"&amp;IF(A113="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C113),"",("('"&amp;FragenTemplate!C113&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D113),"","'"&amp;FragenTemplate!D113&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E113,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F113&amp;"', '"&amp;FragenTemplate!G113&amp;"', '"&amp;FragenTemplate!I113&amp;"', '"&amp;FragenTemplate!K113&amp;"', '"&amp;FragenTemplate!M113&amp;"', "&amp;IF(EXACT(FragenTemplate!H113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L113,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N113,"richtig"),"true","false")&amp;",true)"&amp;IF(A113="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C115),"",("('"&amp;FragenTemplate!C115&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D115),"","'"&amp;FragenTemplate!D115&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E115,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F115&amp;"', '"&amp;FragenTemplate!G115&amp;"', '"&amp;FragenTemplate!I115&amp;"', '"&amp;FragenTemplate!K115&amp;"', '"&amp;FragenTemplate!M115&amp;"', "&amp;IF(EXACT(FragenTemplate!H115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N115,"richtig"),"true","false")&amp;",true)"&amp;IF(A114="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C114),"",("('"&amp;FragenTemplate!C114&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D114),"","'"&amp;FragenTemplate!D114&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E114,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F114&amp;"', '"&amp;FragenTemplate!G114&amp;"', '"&amp;FragenTemplate!I114&amp;"', '"&amp;FragenTemplate!K114&amp;"', '"&amp;FragenTemplate!M114&amp;"', "&amp;IF(EXACT(FragenTemplate!H114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L114,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N114,"richtig"),"true","false")&amp;",true)"&amp;IF(A114="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C116),"",("('"&amp;FragenTemplate!C116&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D116),"","'"&amp;FragenTemplate!D116&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E116,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F116&amp;"', '"&amp;FragenTemplate!G116&amp;"', '"&amp;FragenTemplate!I116&amp;"', '"&amp;FragenTemplate!K116&amp;"', '"&amp;FragenTemplate!M116&amp;"', "&amp;IF(EXACT(FragenTemplate!H116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N116,"richtig"),"true","false")&amp;",true)"&amp;IF(A115="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C115),"",("('"&amp;FragenTemplate!C115&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D115),"","'"&amp;FragenTemplate!D115&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E115,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F115&amp;"', '"&amp;FragenTemplate!G115&amp;"', '"&amp;FragenTemplate!I115&amp;"', '"&amp;FragenTemplate!K115&amp;"', '"&amp;FragenTemplate!M115&amp;"', "&amp;IF(EXACT(FragenTemplate!H115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L115,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N115,"richtig"),"true","false")&amp;",true)"&amp;IF(A115="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C117),"",("('"&amp;FragenTemplate!C117&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D117),"","'"&amp;FragenTemplate!D117&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E117,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F117&amp;"', '"&amp;FragenTemplate!G117&amp;"', '"&amp;FragenTemplate!I117&amp;"', '"&amp;FragenTemplate!K117&amp;"', '"&amp;FragenTemplate!M117&amp;"', "&amp;IF(EXACT(FragenTemplate!H117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N117,"richtig"),"true","false")&amp;",true)"&amp;IF(A116="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C116),"",("('"&amp;FragenTemplate!C116&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D116),"","'"&amp;FragenTemplate!D116&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E116,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F116&amp;"', '"&amp;FragenTemplate!G116&amp;"', '"&amp;FragenTemplate!I116&amp;"', '"&amp;FragenTemplate!K116&amp;"', '"&amp;FragenTemplate!M116&amp;"', "&amp;IF(EXACT(FragenTemplate!H116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L116,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N116,"richtig"),"true","false")&amp;",true)"&amp;IF(A116="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C118),"",("('"&amp;FragenTemplate!C118&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D118),"","'"&amp;FragenTemplate!D118&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E118,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F118&amp;"', '"&amp;FragenTemplate!G118&amp;"', '"&amp;FragenTemplate!I118&amp;"', '"&amp;FragenTemplate!K118&amp;"', '"&amp;FragenTemplate!M118&amp;"', "&amp;IF(EXACT(FragenTemplate!H118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N118,"richtig"),"true","false")&amp;",true)"&amp;IF(A117="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C117),"",("('"&amp;FragenTemplate!C117&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D117),"","'"&amp;FragenTemplate!D117&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E117,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F117&amp;"', '"&amp;FragenTemplate!G117&amp;"', '"&amp;FragenTemplate!I117&amp;"', '"&amp;FragenTemplate!K117&amp;"', '"&amp;FragenTemplate!M117&amp;"', "&amp;IF(EXACT(FragenTemplate!H117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L117,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N117,"richtig"),"true","false")&amp;",true)"&amp;IF(A117="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C119),"",("('"&amp;FragenTemplate!C119&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D119),"","'"&amp;FragenTemplate!D119&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E119,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F119&amp;"', '"&amp;FragenTemplate!G119&amp;"', '"&amp;FragenTemplate!I119&amp;"', '"&amp;FragenTemplate!K119&amp;"', '"&amp;FragenTemplate!M119&amp;"', "&amp;IF(EXACT(FragenTemplate!H119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N119,"richtig"),"true","false")&amp;",true)"&amp;IF(A118="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C118),"",("('"&amp;FragenTemplate!C118&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D118),"","'"&amp;FragenTemplate!D118&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E118,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F118&amp;"', '"&amp;FragenTemplate!G118&amp;"', '"&amp;FragenTemplate!I118&amp;"', '"&amp;FragenTemplate!K118&amp;"', '"&amp;FragenTemplate!M118&amp;"', "&amp;IF(EXACT(FragenTemplate!H118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L118,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N118,"richtig"),"true","false")&amp;",true)"&amp;IF(A118="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C120),"",("('"&amp;FragenTemplate!C120&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D120),"","'"&amp;FragenTemplate!D120&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E120,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F120&amp;"', '"&amp;FragenTemplate!G120&amp;"', '"&amp;FragenTemplate!I120&amp;"', '"&amp;FragenTemplate!K120&amp;"', '"&amp;FragenTemplate!M120&amp;"', "&amp;IF(EXACT(FragenTemplate!H120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N120,"richtig"),"true","false")&amp;",true)"&amp;IF(A119="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C119),"",("('"&amp;FragenTemplate!C119&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D119),"","'"&amp;FragenTemplate!D119&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E119,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F119&amp;"', '"&amp;FragenTemplate!G119&amp;"', '"&amp;FragenTemplate!I119&amp;"', '"&amp;FragenTemplate!K119&amp;"', '"&amp;FragenTemplate!M119&amp;"', "&amp;IF(EXACT(FragenTemplate!H119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L119,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N119,"richtig"),"true","false")&amp;",true)"&amp;IF(A119="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C121),"",("('"&amp;FragenTemplate!C121&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D121),"","'"&amp;FragenTemplate!D121&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E121,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F121&amp;"', '"&amp;FragenTemplate!G121&amp;"', '"&amp;FragenTemplate!I121&amp;"', '"&amp;FragenTemplate!K121&amp;"', '"&amp;FragenTemplate!M121&amp;"', "&amp;IF(EXACT(FragenTemplate!H121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N121,"richtig"),"true","false")&amp;",true)"&amp;IF(A120="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C120),"",("('"&amp;FragenTemplate!C120&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D120),"","'"&amp;FragenTemplate!D120&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E120,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F120&amp;"', '"&amp;FragenTemplate!G120&amp;"', '"&amp;FragenTemplate!I120&amp;"', '"&amp;FragenTemplate!K120&amp;"', '"&amp;FragenTemplate!M120&amp;"', "&amp;IF(EXACT(FragenTemplate!H120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L120,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N120,"richtig"),"true","false")&amp;",true)"&amp;IF(A120="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C122),"",("('"&amp;FragenTemplate!C122&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D122),"","'"&amp;FragenTemplate!D122&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E122,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F122&amp;"', '"&amp;FragenTemplate!G122&amp;"', '"&amp;FragenTemplate!I122&amp;"', '"&amp;FragenTemplate!K122&amp;"', '"&amp;FragenTemplate!M122&amp;"', "&amp;IF(EXACT(FragenTemplate!H122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N122,"richtig"),"true","false")&amp;",true)"&amp;IF(A121="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C121),"",("('"&amp;FragenTemplate!C121&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D121),"","'"&amp;FragenTemplate!D121&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E121,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F121&amp;"', '"&amp;FragenTemplate!G121&amp;"', '"&amp;FragenTemplate!I121&amp;"', '"&amp;FragenTemplate!K121&amp;"', '"&amp;FragenTemplate!M121&amp;"', "&amp;IF(EXACT(FragenTemplate!H121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L121,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N121,"richtig"),"true","false")&amp;",true)"&amp;IF(A121="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C123),"",("('"&amp;FragenTemplate!C123&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D123),"","'"&amp;FragenTemplate!D123&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E123,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F123&amp;"', '"&amp;FragenTemplate!G123&amp;"', '"&amp;FragenTemplate!I123&amp;"', '"&amp;FragenTemplate!K123&amp;"', '"&amp;FragenTemplate!M123&amp;"', "&amp;IF(EXACT(FragenTemplate!H123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N123,"richtig"),"true","false")&amp;",true)"&amp;IF(A122="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C122),"",("('"&amp;FragenTemplate!C122&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D122),"","'"&amp;FragenTemplate!D122&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E122,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F122&amp;"', '"&amp;FragenTemplate!G122&amp;"', '"&amp;FragenTemplate!I122&amp;"', '"&amp;FragenTemplate!K122&amp;"', '"&amp;FragenTemplate!M122&amp;"', "&amp;IF(EXACT(FragenTemplate!H122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L122,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N122,"richtig"),"true","false")&amp;",true)"&amp;IF(A122="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C124),"",("('"&amp;FragenTemplate!C124&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D124),"","'"&amp;FragenTemplate!D124&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E124,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F124&amp;"', '"&amp;FragenTemplate!G124&amp;"', '"&amp;FragenTemplate!I124&amp;"', '"&amp;FragenTemplate!K124&amp;"', '"&amp;FragenTemplate!M124&amp;"', "&amp;IF(EXACT(FragenTemplate!H124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N124,"richtig"),"true","false")&amp;",true)"&amp;IF(A123="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C123),"",("('"&amp;FragenTemplate!C123&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D123),"","'"&amp;FragenTemplate!D123&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E123,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F123&amp;"', '"&amp;FragenTemplate!G123&amp;"', '"&amp;FragenTemplate!I123&amp;"', '"&amp;FragenTemplate!K123&amp;"', '"&amp;FragenTemplate!M123&amp;"', "&amp;IF(EXACT(FragenTemplate!H123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L123,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N123,"richtig"),"true","false")&amp;",true)"&amp;IF(A123="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C125),"",("('"&amp;FragenTemplate!C125&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D125),"","'"&amp;FragenTemplate!D125&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E125,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F125&amp;"', '"&amp;FragenTemplate!G125&amp;"', '"&amp;FragenTemplate!I125&amp;"', '"&amp;FragenTemplate!K125&amp;"', '"&amp;FragenTemplate!M125&amp;"', "&amp;IF(EXACT(FragenTemplate!H125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N125,"richtig"),"true","false")&amp;",true)"&amp;IF(A124="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C124),"",("('"&amp;FragenTemplate!C124&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D124),"","'"&amp;FragenTemplate!D124&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E124,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F124&amp;"', '"&amp;FragenTemplate!G124&amp;"', '"&amp;FragenTemplate!I124&amp;"', '"&amp;FragenTemplate!K124&amp;"', '"&amp;FragenTemplate!M124&amp;"', "&amp;IF(EXACT(FragenTemplate!H124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L124,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N124,"richtig"),"true","false")&amp;",true)"&amp;IF(A124="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C126),"",("('"&amp;FragenTemplate!C126&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D126),"","'"&amp;FragenTemplate!D126&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E126,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F126&amp;"', '"&amp;FragenTemplate!G126&amp;"', '"&amp;FragenTemplate!I126&amp;"', '"&amp;FragenTemplate!K126&amp;"', '"&amp;FragenTemplate!M126&amp;"', "&amp;IF(EXACT(FragenTemplate!H126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N126,"richtig"),"true","false")&amp;",true)"&amp;IF(A125="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C125),"",("('"&amp;FragenTemplate!C125&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D125),"","'"&amp;FragenTemplate!D125&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E125,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F125&amp;"', '"&amp;FragenTemplate!G125&amp;"', '"&amp;FragenTemplate!I125&amp;"', '"&amp;FragenTemplate!K125&amp;"', '"&amp;FragenTemplate!M125&amp;"', "&amp;IF(EXACT(FragenTemplate!H125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L125,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N125,"richtig"),"true","false")&amp;",true)"&amp;IF(A125="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C127),"",("('"&amp;FragenTemplate!C127&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D127),"","'"&amp;FragenTemplate!D127&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E127,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F127&amp;"', '"&amp;FragenTemplate!G127&amp;"', '"&amp;FragenTemplate!I127&amp;"', '"&amp;FragenTemplate!K127&amp;"', '"&amp;FragenTemplate!M127&amp;"', "&amp;IF(EXACT(FragenTemplate!H127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N127,"richtig"),"true","false")&amp;",true)"&amp;IF(A126="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C126),"",("('"&amp;FragenTemplate!C126&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D126),"","'"&amp;FragenTemplate!D126&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E126,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F126&amp;"', '"&amp;FragenTemplate!G126&amp;"', '"&amp;FragenTemplate!I126&amp;"', '"&amp;FragenTemplate!K126&amp;"', '"&amp;FragenTemplate!M126&amp;"', "&amp;IF(EXACT(FragenTemplate!H126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L126,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N126,"richtig"),"true","false")&amp;",true)"&amp;IF(A126="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C128),"",("('"&amp;FragenTemplate!C128&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D128),"","'"&amp;FragenTemplate!D128&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E128,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F128&amp;"', '"&amp;FragenTemplate!G128&amp;"', '"&amp;FragenTemplate!I128&amp;"', '"&amp;FragenTemplate!K128&amp;"', '"&amp;FragenTemplate!M128&amp;"', "&amp;IF(EXACT(FragenTemplate!H128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N128,"richtig"),"true","false")&amp;",true)"&amp;IF(A127="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C127),"",("('"&amp;FragenTemplate!C127&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D127),"","'"&amp;FragenTemplate!D127&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E127,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F127&amp;"', '"&amp;FragenTemplate!G127&amp;"', '"&amp;FragenTemplate!I127&amp;"', '"&amp;FragenTemplate!K127&amp;"', '"&amp;FragenTemplate!M127&amp;"', "&amp;IF(EXACT(FragenTemplate!H127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L127,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N127,"richtig"),"true","false")&amp;",true)"&amp;IF(A127="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C129),"",("('"&amp;FragenTemplate!C129&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D129),"","'"&amp;FragenTemplate!D129&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E129,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F129&amp;"', '"&amp;FragenTemplate!G129&amp;"', '"&amp;FragenTemplate!I129&amp;"', '"&amp;FragenTemplate!K129&amp;"', '"&amp;FragenTemplate!M129&amp;"', "&amp;IF(EXACT(FragenTemplate!H129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N129,"richtig"),"true","false")&amp;",true)"&amp;IF(A128="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C128),"",("('"&amp;FragenTemplate!C128&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D128),"","'"&amp;FragenTemplate!D128&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E128,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F128&amp;"', '"&amp;FragenTemplate!G128&amp;"', '"&amp;FragenTemplate!I128&amp;"', '"&amp;FragenTemplate!K128&amp;"', '"&amp;FragenTemplate!M128&amp;"', "&amp;IF(EXACT(FragenTemplate!H128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L128,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N128,"richtig"),"true","false")&amp;",true)"&amp;IF(A128="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C130),"",("('"&amp;FragenTemplate!C130&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D130),"","'"&amp;FragenTemplate!D130&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E130,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F130&amp;"', '"&amp;FragenTemplate!G130&amp;"', '"&amp;FragenTemplate!I130&amp;"', '"&amp;FragenTemplate!K130&amp;"', '"&amp;FragenTemplate!M130&amp;"', "&amp;IF(EXACT(FragenTemplate!H130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N130,"richtig"),"true","false")&amp;",true)"&amp;IF(A129="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C129),"",("('"&amp;FragenTemplate!C129&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D129),"","'"&amp;FragenTemplate!D129&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E129,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F129&amp;"', '"&amp;FragenTemplate!G129&amp;"', '"&amp;FragenTemplate!I129&amp;"', '"&amp;FragenTemplate!K129&amp;"', '"&amp;FragenTemplate!M129&amp;"', "&amp;IF(EXACT(FragenTemplate!H129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L129,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N129,"richtig"),"true","false")&amp;",true)"&amp;IF(A129="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C131),"",("('"&amp;FragenTemplate!C131&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D131),"","'"&amp;FragenTemplate!D131&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E131,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F131&amp;"', '"&amp;FragenTemplate!G131&amp;"', '"&amp;FragenTemplate!I131&amp;"', '"&amp;FragenTemplate!K131&amp;"', '"&amp;FragenTemplate!M131&amp;"', "&amp;IF(EXACT(FragenTemplate!H131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N131,"richtig"),"true","false")&amp;",true)"&amp;IF(A130="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C130),"",("('"&amp;FragenTemplate!C130&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D130),"","'"&amp;FragenTemplate!D130&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E130,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F130&amp;"', '"&amp;FragenTemplate!G130&amp;"', '"&amp;FragenTemplate!I130&amp;"', '"&amp;FragenTemplate!K130&amp;"', '"&amp;FragenTemplate!M130&amp;"', "&amp;IF(EXACT(FragenTemplate!H130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L130,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N130,"richtig"),"true","false")&amp;",true)"&amp;IF(A130="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C132),"",("('"&amp;FragenTemplate!C132&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D132),"","'"&amp;FragenTemplate!D132&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E132,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F132&amp;"', '"&amp;FragenTemplate!G132&amp;"', '"&amp;FragenTemplate!I132&amp;"', '"&amp;FragenTemplate!K132&amp;"', '"&amp;FragenTemplate!M132&amp;"', "&amp;IF(EXACT(FragenTemplate!H132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N132,"richtig"),"true","false")&amp;",true)"&amp;IF(A131="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C131),"",("('"&amp;FragenTemplate!C131&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D131),"","'"&amp;FragenTemplate!D131&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E131,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F131&amp;"', '"&amp;FragenTemplate!G131&amp;"', '"&amp;FragenTemplate!I131&amp;"', '"&amp;FragenTemplate!K131&amp;"', '"&amp;FragenTemplate!M131&amp;"', "&amp;IF(EXACT(FragenTemplate!H131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L131,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N131,"richtig"),"true","false")&amp;",true)"&amp;IF(A131="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C133),"",("('"&amp;FragenTemplate!C133&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D133),"","'"&amp;FragenTemplate!D133&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E133,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F133&amp;"', '"&amp;FragenTemplate!G133&amp;"', '"&amp;FragenTemplate!I133&amp;"', '"&amp;FragenTemplate!K133&amp;"', '"&amp;FragenTemplate!M133&amp;"', "&amp;IF(EXACT(FragenTemplate!H133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N133,"richtig"),"true","false")&amp;",true)"&amp;IF(A132="",";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C132),"",("('"&amp;FragenTemplate!C132&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D132),"","'"&amp;FragenTemplate!D132&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E132,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F132&amp;"', '"&amp;FragenTemplate!G132&amp;"', '"&amp;FragenTemplate!I132&amp;"', '"&amp;FragenTemplate!K132&amp;"', '"&amp;FragenTemplate!M132&amp;"', "&amp;IF(EXACT(FragenTemplate!H132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L132,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N132,"richtig"),"true","false")&amp;",true)"&amp;IF(A132="",";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C134),"",("('"&amp;FragenTemplate!C134&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D134),"","'"&amp;FragenTemplate!D134&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E134,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F134&amp;"', '"&amp;FragenTemplate!G134&amp;"', '"&amp;FragenTemplate!I134&amp;"', '"&amp;FragenTemplate!K134&amp;"', '"&amp;FragenTemplate!M134&amp;"', "&amp;IF(EXACT(FragenTemplate!H134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N134,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A133),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C133),"",("('"&amp;FragenTemplate!C133&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D133),"","'"&amp;FragenTemplate!D133&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E133,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F133&amp;"', '"&amp;FragenTemplate!G133&amp;"', '"&amp;FragenTemplate!I133&amp;"', '"&amp;FragenTemplate!K133&amp;"', '"&amp;FragenTemplate!M133&amp;"', "&amp;IF(EXACT(FragenTemplate!H133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L133,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N133,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A133),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C135),"",("('"&amp;FragenTemplate!C135&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D135),"","'"&amp;FragenTemplate!D135&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E135,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F135&amp;"', '"&amp;FragenTemplate!G135&amp;"', '"&amp;FragenTemplate!I135&amp;"', '"&amp;FragenTemplate!K135&amp;"', '"&amp;FragenTemplate!M135&amp;"', "&amp;IF(EXACT(FragenTemplate!H135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N135,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A134),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C134),"",("('"&amp;FragenTemplate!C134&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D134),"","'"&amp;FragenTemplate!D134&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E134,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F134&amp;"', '"&amp;FragenTemplate!G134&amp;"', '"&amp;FragenTemplate!I134&amp;"', '"&amp;FragenTemplate!K134&amp;"', '"&amp;FragenTemplate!M134&amp;"', "&amp;IF(EXACT(FragenTemplate!H134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L134,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N134,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A134),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C136),"",("('"&amp;FragenTemplate!C136&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D136),"","'"&amp;FragenTemplate!D136&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E136,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F136&amp;"', '"&amp;FragenTemplate!G136&amp;"', '"&amp;FragenTemplate!I136&amp;"', '"&amp;FragenTemplate!K136&amp;"', '"&amp;FragenTemplate!M136&amp;"', "&amp;IF(EXACT(FragenTemplate!H136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N136,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A135),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C135),"",("('"&amp;FragenTemplate!C135&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D135),"","'"&amp;FragenTemplate!D135&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E135,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F135&amp;"', '"&amp;FragenTemplate!G135&amp;"', '"&amp;FragenTemplate!I135&amp;"', '"&amp;FragenTemplate!K135&amp;"', '"&amp;FragenTemplate!M135&amp;"', "&amp;IF(EXACT(FragenTemplate!H135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L135,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N135,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A135),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C137),"",("('"&amp;FragenTemplate!C137&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D137),"","'"&amp;FragenTemplate!D137&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E137,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F137&amp;"', '"&amp;FragenTemplate!G137&amp;"', '"&amp;FragenTemplate!I137&amp;"', '"&amp;FragenTemplate!K137&amp;"', '"&amp;FragenTemplate!M137&amp;"', "&amp;IF(EXACT(FragenTemplate!H137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N137,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A136),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C136),"",("('"&amp;FragenTemplate!C136&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D136),"","'"&amp;FragenTemplate!D136&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E136,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F136&amp;"', '"&amp;FragenTemplate!G136&amp;"', '"&amp;FragenTemplate!I136&amp;"', '"&amp;FragenTemplate!K136&amp;"', '"&amp;FragenTemplate!M136&amp;"', "&amp;IF(EXACT(FragenTemplate!H136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L136,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N136,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A136),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C138),"",("('"&amp;FragenTemplate!C138&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D138),"","'"&amp;FragenTemplate!D138&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E138,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F138&amp;"', '"&amp;FragenTemplate!G138&amp;"', '"&amp;FragenTemplate!I138&amp;"', '"&amp;FragenTemplate!K138&amp;"', '"&amp;FragenTemplate!M138&amp;"', "&amp;IF(EXACT(FragenTemplate!H138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N138,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A137),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C137),"",("('"&amp;FragenTemplate!C137&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D137),"","'"&amp;FragenTemplate!D137&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E137,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F137&amp;"', '"&amp;FragenTemplate!G137&amp;"', '"&amp;FragenTemplate!I137&amp;"', '"&amp;FragenTemplate!K137&amp;"', '"&amp;FragenTemplate!M137&amp;"', "&amp;IF(EXACT(FragenTemplate!H137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L137,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N137,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A137),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C139),"",("('"&amp;FragenTemplate!C139&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D139),"","'"&amp;FragenTemplate!D139&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E139,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F139&amp;"', '"&amp;FragenTemplate!G139&amp;"', '"&amp;FragenTemplate!I139&amp;"', '"&amp;FragenTemplate!K139&amp;"', '"&amp;FragenTemplate!M139&amp;"', "&amp;IF(EXACT(FragenTemplate!H139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N139,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A138),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C138),"",("('"&amp;FragenTemplate!C138&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D138),"","'"&amp;FragenTemplate!D138&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E138,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F138&amp;"', '"&amp;FragenTemplate!G138&amp;"', '"&amp;FragenTemplate!I138&amp;"', '"&amp;FragenTemplate!K138&amp;"', '"&amp;FragenTemplate!M138&amp;"', "&amp;IF(EXACT(FragenTemplate!H138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L138,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N138,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A138),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C140),"",("('"&amp;FragenTemplate!C140&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D140),"","'"&amp;FragenTemplate!D140&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E140,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F140&amp;"', '"&amp;FragenTemplate!G140&amp;"', '"&amp;FragenTemplate!I140&amp;"', '"&amp;FragenTemplate!K140&amp;"', '"&amp;FragenTemplate!M140&amp;"', "&amp;IF(EXACT(FragenTemplate!H140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N140,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A139),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C139),"",("('"&amp;FragenTemplate!C139&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D139),"","'"&amp;FragenTemplate!D139&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E139,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F139&amp;"', '"&amp;FragenTemplate!G139&amp;"', '"&amp;FragenTemplate!I139&amp;"', '"&amp;FragenTemplate!K139&amp;"', '"&amp;FragenTemplate!M139&amp;"', "&amp;IF(EXACT(FragenTemplate!H139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L139,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N139,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A139),";",",")))</f>
         <v/>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
-        <f>IF(ISBLANK(FragenTemplate!C141),"",("('"&amp;FragenTemplate!C141&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D141),"","'"&amp;FragenTemplate!D141&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E141,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F141&amp;"', '"&amp;FragenTemplate!G141&amp;"', '"&amp;FragenTemplate!I141&amp;"', '"&amp;FragenTemplate!K141&amp;"', '"&amp;FragenTemplate!M141&amp;"', "&amp;IF(EXACT(FragenTemplate!H141,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J141,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L141,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N141,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A140),";",",")))</f>
+        <f>IF(ISBLANK(FragenTemplate!C140),"",("('"&amp;FragenTemplate!C140&amp;"', "&amp;IF(ISBLANK(FragenTemplate!D140),"","'"&amp;FragenTemplate!D140&amp;"'")&amp;", "&amp;IF(EXACT(FragenTemplate!E140,"richtig"),"true","false")&amp;", '"&amp;FragenTemplate!F140&amp;"', '"&amp;FragenTemplate!G140&amp;"', '"&amp;FragenTemplate!I140&amp;"', '"&amp;FragenTemplate!K140&amp;"', '"&amp;FragenTemplate!M140&amp;"', "&amp;IF(EXACT(FragenTemplate!H140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!J140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!L140,"richtig"),"true","false")&amp;","&amp;IF(EXACT(FragenTemplate!N140,"richtig"),"true","false")&amp;",true)"&amp;IF(ISBLANK(A140),";",",")))</f>
         <v/>
       </c>
     </row>

</xml_diff>